<commit_message>
feat(i18n): generate structured locale
</commit_message>
<xml_diff>
--- a/scripts/i18n.xlsx
+++ b/scripts/i18n.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
   <authors>
     <author/>
   </authors>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1149" uniqueCount="613">
   <si>
     <t xml:space="preserve">페이지는 [피그마] PFPlay GUI 설계서 합본의 페이지 이름입니다. </t>
   </si>
@@ -952,11 +952,11 @@
     <t>[팝업2] 플레이리스트에 존재 시</t>
   </si>
   <si>
-    <t>namename'에 이미 존재하는 곡입니다! 
+    <t>$1'에 이미 존재하는 곡입니다! 
 중복곡은 삭제하고 다시 담을까요?</t>
   </si>
   <si>
-    <t>namename' already has this song! Shall we delete the duplicate song and put it back?</t>
+    <t>$1' already has this song! Shall we delete the duplicate song and put it back?</t>
   </si>
   <si>
     <t>namename' already has this song! Should we remove the duplicate and add it again?</t>
@@ -1531,6 +1531,15 @@
     <t>common.btn.eng</t>
   </si>
   <si>
+    <t>common.btn.enter_again</t>
+  </si>
+  <si>
+    <t>다시 입장하기</t>
+  </si>
+  <si>
+    <t>Try again</t>
+  </si>
+  <si>
     <t>Error Case</t>
   </si>
   <si>
@@ -1903,38 +1912,128 @@
     <t>playlist.para.search_url</t>
   </si>
   <si>
+    <t>playlist.para.up_to_10_if_connect_wallet</t>
+  </si>
+  <si>
+    <t>지갑을 연동하시면 10개까지 생성할 수 있어요!</t>
+  </si>
+  <si>
+    <t>If you connect your wallet, you can create up to 10!</t>
+  </si>
+  <si>
     <t>playlist.ec.exceeded_list_connect_wallet</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">이미 생성 가능한 리스트 수를 초과했어요.
+    <t xml:space="preserve">이미 생성 가능한 리스트 수를 초과했어요.
 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-        <u/>
-      </rPr>
-      <t>지갑을 연동하시면</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve"> 10개까지 생성할 수 있어요!</t>
-    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">You have already exceeded the number of lists that can be created. </t>
   </si>
   <si>
     <t>playlist.ec.exceeded_list</t>
   </si>
   <si>
+    <t>이런! 생성 가능한 리스트 수를 초과했어요\n최대 10개 까지만 생성이 가능해요</t>
+  </si>
+  <si>
     <t>playlist.ec.up_to_100_songs</t>
+  </si>
+  <si>
+    <t>파티룸 입장(Partyroom)</t>
+  </si>
+  <si>
+    <t>Loading</t>
+  </si>
+  <si>
+    <t>partyroom.loading.text_1</t>
+  </si>
+  <si>
+    <t>로딩페이지 문구 1</t>
+  </si>
+  <si>
+    <t>en-로딩페이지 문구 1</t>
+  </si>
+  <si>
+    <t>partyroom.loading.text_2</t>
+  </si>
+  <si>
+    <t>로딩페이지 문구 2</t>
+  </si>
+  <si>
+    <t>en-로딩페이지 문구 2</t>
+  </si>
+  <si>
+    <t>partyroom.loading.text_3</t>
+  </si>
+  <si>
+    <t>로딩페이지 문구 3</t>
+  </si>
+  <si>
+    <t>en-로딩페이지 문구 3</t>
+  </si>
+  <si>
+    <t>partyroom.loading.text_4</t>
+  </si>
+  <si>
+    <t>로딩페이지 문구 4</t>
+  </si>
+  <si>
+    <t>en-로딩페이지 문구 4</t>
+  </si>
+  <si>
+    <t>partyroom.loading.text_5</t>
+  </si>
+  <si>
+    <t>로딩페이지 문구 5</t>
+  </si>
+  <si>
+    <t>en-로딩페이지 문구 5</t>
+  </si>
+  <si>
+    <t>partyroom.loading.text_6</t>
+  </si>
+  <si>
+    <t>로딩페이지 문구 6</t>
+  </si>
+  <si>
+    <t>en-로딩페이지 문구 6</t>
+  </si>
+  <si>
+    <t>partyroom.loading.text_7</t>
+  </si>
+  <si>
+    <t>로딩페이지 문구 7</t>
+  </si>
+  <si>
+    <t>en-로딩페이지 문구 7</t>
+  </si>
+  <si>
+    <t>partyroom.loading.text_8</t>
+  </si>
+  <si>
+    <t>로딩페이지 문구 8</t>
+  </si>
+  <si>
+    <t>en-로딩페이지 문구 8</t>
+  </si>
+  <si>
+    <t>partyroom.ec.shut_down</t>
+  </si>
+  <si>
+    <t>더 이상 존재하지 않는 파티룸이에요</t>
+  </si>
+  <si>
+    <t>en-더 이상 존재하지 않는 파티룸이에요</t>
+  </si>
+  <si>
+    <t>partyroom.ec.data_load</t>
+  </si>
+  <si>
+    <t>데이터를 불러오는데 실패했습니다.\n다시 입장하시겠어요?</t>
+  </si>
+  <si>
+    <t>en-데이터를 불러오는데 실패했습니다.\n다시 입장하시겠어요?</t>
   </si>
 </sst>
 </file>
@@ -5424,14 +5523,14 @@
     <mergeCell ref="B36:B41"/>
     <mergeCell ref="A46:A64"/>
     <mergeCell ref="B106:B110"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:D2"/>
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="A12:A29"/>
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:D2"/>
     <mergeCell ref="B46:B48"/>
     <mergeCell ref="B49:B64"/>
     <mergeCell ref="B71:B86"/>
@@ -5990,31 +6089,31 @@
       <c r="H34" s="17"/>
     </row>
     <row r="35">
-      <c r="B35" s="15" t="s">
+      <c r="C35" s="21" t="s">
         <v>445</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="D35" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="E35" s="3" t="s">
-        <v>39</v>
+        <v>447</v>
       </c>
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
       <c r="H35" s="17"/>
     </row>
     <row r="36">
-      <c r="C36" s="8" t="s">
-        <v>447</v>
+      <c r="B36" s="15" t="s">
+        <v>448</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>449</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F36" s="17"/>
       <c r="G36" s="18"/>
@@ -6022,13 +6121,13 @@
     </row>
     <row r="37">
       <c r="C37" s="8" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>242</v>
+        <v>43</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>243</v>
+        <v>44</v>
       </c>
       <c r="F37" s="17"/>
       <c r="G37" s="18"/>
@@ -6036,47 +6135,47 @@
     </row>
     <row r="38">
       <c r="C38" s="8" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>301</v>
+        <v>242</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>302</v>
+        <v>243</v>
       </c>
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
       <c r="H38" s="17"/>
     </row>
     <row r="39">
-      <c r="A39" s="15" t="s">
-        <v>450</v>
-      </c>
-      <c r="B39" s="21" t="s">
-        <v>451</v>
-      </c>
-      <c r="C39" s="15" t="s">
+      <c r="C39" s="8" t="s">
         <v>452</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>136</v>
+        <v>301</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>137</v>
+        <v>302</v>
       </c>
       <c r="F39" s="17"/>
       <c r="G39" s="18"/>
       <c r="H39" s="17"/>
     </row>
     <row r="40">
+      <c r="A40" s="15" t="s">
+        <v>453</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>454</v>
+      </c>
       <c r="C40" s="15" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F40" s="17"/>
       <c r="G40" s="18"/>
@@ -6084,27 +6183,27 @@
     </row>
     <row r="41">
       <c r="C41" s="15" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="F41" s="17"/>
       <c r="G41" s="18"/>
       <c r="H41" s="17"/>
     </row>
     <row r="42">
-      <c r="C42" s="21" t="s">
-        <v>455</v>
+      <c r="C42" s="15" t="s">
+        <v>457</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="F42" s="17"/>
       <c r="G42" s="18"/>
@@ -6112,13 +6211,13 @@
     </row>
     <row r="43">
       <c r="C43" s="21" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>194</v>
+        <v>132</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>195</v>
+        <v>133</v>
       </c>
       <c r="F43" s="17"/>
       <c r="G43" s="18"/>
@@ -6126,13 +6225,13 @@
     </row>
     <row r="44">
       <c r="C44" s="21" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="18"/>
@@ -6140,13 +6239,13 @@
     </row>
     <row r="45">
       <c r="C45" s="21" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="F45" s="17"/>
       <c r="G45" s="18"/>
@@ -6154,13 +6253,13 @@
     </row>
     <row r="46">
       <c r="C46" s="21" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>331</v>
+        <v>204</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>332</v>
+        <v>205</v>
       </c>
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
@@ -6168,13 +6267,13 @@
     </row>
     <row r="47">
       <c r="C47" s="21" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>336</v>
+        <v>331</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>332</v>
       </c>
       <c r="F47" s="17"/>
       <c r="G47" s="18"/>
@@ -6182,75 +6281,75 @@
     </row>
     <row r="48">
       <c r="C48" s="21" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="F48" s="17"/>
       <c r="G48" s="18"/>
       <c r="H48" s="17"/>
     </row>
     <row r="49">
-      <c r="B49" s="21" t="s">
-        <v>413</v>
-      </c>
       <c r="C49" s="21" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>59</v>
+        <v>339</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>340</v>
       </c>
       <c r="F49" s="17"/>
       <c r="G49" s="18"/>
       <c r="H49" s="17"/>
     </row>
     <row r="50">
+      <c r="B50" s="21" t="s">
+        <v>413</v>
+      </c>
       <c r="C50" s="21" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>29</v>
+        <v>250</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="F50" s="17"/>
       <c r="G50" s="18"/>
       <c r="H50" s="17"/>
     </row>
     <row r="51">
-      <c r="B51" s="21" t="s">
-        <v>464</v>
-      </c>
       <c r="C51" s="21" t="s">
-        <v>465</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>321</v>
+        <v>466</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>322</v>
+        <v>30</v>
       </c>
       <c r="F51" s="17"/>
       <c r="G51" s="18"/>
       <c r="H51" s="17"/>
     </row>
     <row r="52">
+      <c r="B52" s="21" t="s">
+        <v>467</v>
+      </c>
       <c r="C52" s="21" t="s">
-        <v>466</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>324</v>
+        <v>468</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>321</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="F52" s="17"/>
       <c r="G52" s="18"/>
@@ -6258,13 +6357,13 @@
     </row>
     <row r="53">
       <c r="C53" s="21" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="18"/>
@@ -6272,13 +6371,13 @@
     </row>
     <row r="54">
       <c r="C54" s="21" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F54" s="17"/>
       <c r="G54" s="18"/>
@@ -6286,13 +6385,13 @@
     </row>
     <row r="55">
       <c r="C55" s="21" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="18"/>
@@ -6300,13 +6399,13 @@
     </row>
     <row r="56">
       <c r="C56" s="21" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F56" s="17"/>
       <c r="G56" s="18"/>
@@ -6314,47 +6413,47 @@
     </row>
     <row r="57">
       <c r="C57" s="21" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>190</v>
+        <v>329</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>191</v>
+        <v>329</v>
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="18"/>
       <c r="H57" s="17"/>
     </row>
     <row r="58">
-      <c r="A58" s="21" t="s">
-        <v>472</v>
-      </c>
-      <c r="B58" s="21" t="s">
-        <v>413</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>473</v>
+      <c r="C58" s="21" t="s">
+        <v>474</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>11</v>
+        <v>190</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>11</v>
+        <v>191</v>
       </c>
       <c r="F58" s="17"/>
       <c r="G58" s="18"/>
       <c r="H58" s="17"/>
     </row>
     <row r="59">
-      <c r="C59" s="21" t="s">
-        <v>474</v>
+      <c r="A59" s="21" t="s">
+        <v>475</v>
+      </c>
+      <c r="B59" s="21" t="s">
+        <v>413</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>476</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E59" s="5" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="F59" s="17"/>
       <c r="G59" s="18"/>
@@ -6362,13 +6461,13 @@
     </row>
     <row r="60">
       <c r="C60" s="21" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="F60" s="17"/>
       <c r="G60" s="18"/>
@@ -6376,13 +6475,13 @@
     </row>
     <row r="61">
       <c r="C61" s="21" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F61" s="17"/>
       <c r="G61" s="18"/>
@@ -6390,13 +6489,13 @@
     </row>
     <row r="62">
       <c r="C62" s="21" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F62" s="17"/>
       <c r="G62" s="18"/>
@@ -6404,30 +6503,27 @@
     </row>
     <row r="63">
       <c r="C63" s="21" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="F63" s="17"/>
       <c r="G63" s="18"/>
       <c r="H63" s="17"/>
     </row>
     <row r="64">
-      <c r="B64" s="21" t="s">
-        <v>464</v>
-      </c>
       <c r="C64" s="21" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="F64" s="17"/>
       <c r="G64" s="18"/>
@@ -6435,50 +6531,53 @@
     </row>
     <row r="65">
       <c r="B65" s="21" t="s">
-        <v>451</v>
+        <v>467</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F65" s="17"/>
       <c r="G65" s="18"/>
       <c r="H65" s="17"/>
     </row>
     <row r="66">
-      <c r="A66" s="21" t="s">
-        <v>481</v>
-      </c>
       <c r="B66" s="21" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F66" s="17"/>
       <c r="G66" s="18"/>
       <c r="H66" s="17"/>
     </row>
     <row r="67">
+      <c r="A67" s="21" t="s">
+        <v>484</v>
+      </c>
+      <c r="B67" s="21" t="s">
+        <v>467</v>
+      </c>
       <c r="C67" s="21" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F67" s="17"/>
       <c r="G67" s="18"/>
@@ -6486,13 +6585,13 @@
     </row>
     <row r="68">
       <c r="C68" s="21" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>485</v>
+        <v>37</v>
       </c>
       <c r="F68" s="17"/>
       <c r="G68" s="18"/>
@@ -6500,13 +6599,13 @@
     </row>
     <row r="69">
       <c r="C69" s="21" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>50</v>
+        <v>488</v>
       </c>
       <c r="F69" s="17"/>
       <c r="G69" s="18"/>
@@ -6514,13 +6613,13 @@
     </row>
     <row r="70">
       <c r="C70" s="21" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F70" s="17"/>
       <c r="G70" s="18"/>
@@ -6528,13 +6627,13 @@
     </row>
     <row r="71">
       <c r="C71" s="21" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F71" s="17"/>
       <c r="G71" s="18"/>
@@ -6542,30 +6641,27 @@
     </row>
     <row r="72">
       <c r="C72" s="21" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F72" s="17"/>
       <c r="G72" s="18"/>
       <c r="H72" s="17"/>
     </row>
     <row r="73">
-      <c r="B73" s="21" t="s">
-        <v>445</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>490</v>
+      <c r="C73" s="21" t="s">
+        <v>492</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="F73" s="17"/>
       <c r="G73" s="18"/>
@@ -6573,16 +6669,16 @@
     </row>
     <row r="74">
       <c r="B74" s="21" t="s">
-        <v>413</v>
+        <v>448</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F74" s="17"/>
       <c r="G74" s="18"/>
@@ -6590,64 +6686,67 @@
     </row>
     <row r="75">
       <c r="B75" s="21" t="s">
-        <v>451</v>
+        <v>413</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="F75" s="17"/>
       <c r="G75" s="18"/>
       <c r="H75" s="17"/>
     </row>
     <row r="76">
+      <c r="B76" s="21" t="s">
+        <v>454</v>
+      </c>
       <c r="C76" s="3" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="D76" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F76" s="17"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="17"/>
+    </row>
+    <row r="77">
+      <c r="C77" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="D77" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E77" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F76" s="24"/>
-      <c r="G76" s="24"/>
-      <c r="H76" s="24"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="21" t="s">
-        <v>494</v>
-      </c>
-      <c r="B77" s="25" t="s">
-        <v>464</v>
-      </c>
-      <c r="C77" s="21" t="s">
-        <v>495</v>
-      </c>
-      <c r="D77" s="3" t="s">
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="24"/>
+    </row>
+    <row r="78">
+      <c r="A78" s="21" t="s">
+        <v>497</v>
+      </c>
+      <c r="B78" s="25" t="s">
+        <v>467</v>
+      </c>
+      <c r="C78" s="21" t="s">
+        <v>498</v>
+      </c>
+      <c r="D78" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E77" s="3" t="s">
+      <c r="E78" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="F77" s="17"/>
-      <c r="G77" s="18"/>
-      <c r="H77" s="17"/>
-    </row>
-    <row r="78">
-      <c r="C78" s="21" t="s">
-        <v>496</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="E78" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="F78" s="17"/>
       <c r="G78" s="18"/>
@@ -6655,13 +6754,13 @@
     </row>
     <row r="79">
       <c r="C79" s="21" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F79" s="17"/>
       <c r="G79" s="18"/>
@@ -6669,79 +6768,78 @@
     </row>
     <row r="80">
       <c r="C80" s="21" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F80" s="17"/>
       <c r="G80" s="18"/>
       <c r="H80" s="17"/>
     </row>
     <row r="81">
-      <c r="B81" s="21" t="s">
-        <v>451</v>
-      </c>
       <c r="C81" s="21" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>79</v>
+        <v>104</v>
       </c>
       <c r="F81" s="17"/>
       <c r="G81" s="18"/>
       <c r="H81" s="17"/>
     </row>
     <row r="82">
-      <c r="A82" s="21" t="s">
-        <v>500</v>
-      </c>
       <c r="B82" s="21" t="s">
-        <v>464</v>
+        <v>454</v>
       </c>
       <c r="C82" s="21" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D82" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E82" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F82" s="17"/>
+      <c r="G82" s="18"/>
+      <c r="H82" s="17"/>
+    </row>
+    <row r="83">
+      <c r="A83" s="21" t="s">
+        <v>503</v>
+      </c>
+      <c r="B83" s="21" t="s">
+        <v>467</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>504</v>
+      </c>
+      <c r="D83" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="E82" s="3" t="s">
+      <c r="E83" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="F82" s="24"/>
-      <c r="G82" s="24"/>
-      <c r="H82" s="24"/>
-    </row>
-    <row r="83">
-      <c r="C83" s="21" t="s">
-        <v>502</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="E83" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="F83" s="24"/>
       <c r="G83" s="24"/>
       <c r="H83" s="24"/>
     </row>
     <row r="84">
-      <c r="B84" s="21"/>
       <c r="C84" s="21" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="F84" s="24"/>
       <c r="G84" s="24"/>
@@ -6750,44 +6848,45 @@
     <row r="85">
       <c r="B85" s="21"/>
       <c r="C85" s="21" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F85" s="24"/>
       <c r="G85" s="24"/>
       <c r="H85" s="24"/>
     </row>
     <row r="86">
-      <c r="B86" s="21" t="s">
-        <v>451</v>
-      </c>
+      <c r="B86" s="21"/>
       <c r="C86" s="21" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>108</v>
+        <v>156</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>109</v>
+        <v>157</v>
       </c>
       <c r="F86" s="24"/>
       <c r="G86" s="24"/>
       <c r="H86" s="24"/>
     </row>
     <row r="87">
+      <c r="B87" s="21" t="s">
+        <v>454</v>
+      </c>
       <c r="C87" s="21" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F87" s="24"/>
       <c r="G87" s="24"/>
@@ -6795,13 +6894,13 @@
     </row>
     <row r="88">
       <c r="C88" s="21" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>168</v>
+        <v>110</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>169</v>
+        <v>111</v>
       </c>
       <c r="F88" s="24"/>
       <c r="G88" s="24"/>
@@ -6809,13 +6908,13 @@
     </row>
     <row r="89">
       <c r="C89" s="21" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F89" s="24"/>
       <c r="G89" s="24"/>
@@ -6823,13 +6922,13 @@
     </row>
     <row r="90">
       <c r="C90" s="21" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="F90" s="24"/>
       <c r="G90" s="24"/>
@@ -6837,13 +6936,13 @@
     </row>
     <row r="91">
       <c r="C91" s="21" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="E91" s="3" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F91" s="24"/>
       <c r="G91" s="24"/>
@@ -6851,13 +6950,13 @@
     </row>
     <row r="92">
       <c r="C92" s="21" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>209</v>
+        <v>183</v>
       </c>
       <c r="F92" s="24"/>
       <c r="G92" s="24"/>
@@ -6865,13 +6964,13 @@
     </row>
     <row r="93">
       <c r="C93" s="21" t="s">
-        <v>512</v>
-      </c>
-      <c r="D93" s="9" t="s">
-        <v>211</v>
+        <v>514</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F93" s="24"/>
       <c r="G93" s="24"/>
@@ -6879,13 +6978,13 @@
     </row>
     <row r="94">
       <c r="C94" s="21" t="s">
-        <v>513</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>312</v>
+        <v>515</v>
+      </c>
+      <c r="D94" s="9" t="s">
+        <v>211</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>313</v>
+        <v>212</v>
       </c>
       <c r="F94" s="24"/>
       <c r="G94" s="24"/>
@@ -6893,13 +6992,13 @@
     </row>
     <row r="95">
       <c r="C95" s="21" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>306</v>
+        <v>312</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="F95" s="24"/>
       <c r="G95" s="24"/>
@@ -6907,13 +7006,13 @@
     </row>
     <row r="96">
       <c r="C96" s="21" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>221</v>
+        <v>306</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>222</v>
+        <v>306</v>
       </c>
       <c r="F96" s="24"/>
       <c r="G96" s="24"/>
@@ -6921,13 +7020,13 @@
     </row>
     <row r="97">
       <c r="C97" s="21" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="F97" s="24"/>
       <c r="G97" s="24"/>
@@ -6935,78 +7034,78 @@
     </row>
     <row r="98">
       <c r="C98" s="21" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F98" s="24"/>
       <c r="G98" s="24"/>
       <c r="H98" s="24"/>
     </row>
     <row r="99">
-      <c r="B99" s="21" t="s">
-        <v>413</v>
-      </c>
       <c r="C99" s="21" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>178</v>
+        <v>216</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>179</v>
+        <v>217</v>
       </c>
       <c r="F99" s="24"/>
       <c r="G99" s="24"/>
       <c r="H99" s="24"/>
     </row>
     <row r="100">
+      <c r="B100" s="21" t="s">
+        <v>413</v>
+      </c>
       <c r="C100" s="21" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F100" s="24"/>
       <c r="G100" s="24"/>
       <c r="H100" s="24"/>
     </row>
     <row r="101">
-      <c r="A101" s="15" t="s">
-        <v>520</v>
-      </c>
-      <c r="B101" s="15" t="s">
-        <v>464</v>
-      </c>
-      <c r="C101" s="15" t="s">
-        <v>521</v>
+      <c r="C101" s="21" t="s">
+        <v>522</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>144</v>
+        <v>180</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>344</v>
+        <v>181</v>
       </c>
       <c r="F101" s="24"/>
       <c r="G101" s="24"/>
       <c r="H101" s="24"/>
     </row>
     <row r="102">
+      <c r="A102" s="15" t="s">
+        <v>523</v>
+      </c>
+      <c r="B102" s="15" t="s">
+        <v>467</v>
+      </c>
       <c r="C102" s="15" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>116</v>
+        <v>144</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>117</v>
+        <v>344</v>
       </c>
       <c r="F102" s="24"/>
       <c r="G102" s="24"/>
@@ -7014,41 +7113,41 @@
     </row>
     <row r="103">
       <c r="C103" s="15" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>351</v>
+        <v>116</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>352</v>
+        <v>117</v>
       </c>
       <c r="F103" s="24"/>
       <c r="G103" s="24"/>
       <c r="H103" s="24"/>
     </row>
     <row r="104">
-      <c r="C104" s="21" t="s">
-        <v>524</v>
+      <c r="C104" s="15" t="s">
+        <v>526</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>385</v>
+        <v>351</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>386</v>
+        <v>352</v>
       </c>
       <c r="F104" s="24"/>
       <c r="G104" s="24"/>
       <c r="H104" s="24"/>
     </row>
     <row r="105">
-      <c r="C105" s="15" t="s">
-        <v>525</v>
+      <c r="C105" s="21" t="s">
+        <v>527</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>146</v>
+        <v>385</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>147</v>
+        <v>386</v>
       </c>
       <c r="F105" s="24"/>
       <c r="G105" s="24"/>
@@ -7056,13 +7155,13 @@
     </row>
     <row r="106">
       <c r="C106" s="15" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="F106" s="24"/>
       <c r="G106" s="24"/>
@@ -7070,13 +7169,13 @@
     </row>
     <row r="107">
       <c r="C107" s="15" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F107" s="24"/>
       <c r="G107" s="24"/>
@@ -7084,13 +7183,13 @@
     </row>
     <row r="108">
       <c r="C108" s="15" t="s">
-        <v>528</v>
-      </c>
-      <c r="D108" s="7" t="s">
-        <v>163</v>
+        <v>530</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F108" s="24"/>
       <c r="G108" s="24"/>
@@ -7098,103 +7197,103 @@
     </row>
     <row r="109">
       <c r="C109" s="15" t="s">
-        <v>529</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>123</v>
+        <v>531</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>163</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>124</v>
+        <v>164</v>
       </c>
       <c r="F109" s="24"/>
       <c r="G109" s="24"/>
       <c r="H109" s="24"/>
     </row>
     <row r="110">
-      <c r="B110" s="15" t="s">
-        <v>413</v>
-      </c>
       <c r="C110" s="15" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>348</v>
+        <v>123</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>349</v>
+        <v>124</v>
       </c>
       <c r="F110" s="24"/>
       <c r="G110" s="24"/>
       <c r="H110" s="24"/>
     </row>
     <row r="111">
+      <c r="B111" s="15" t="s">
+        <v>413</v>
+      </c>
       <c r="C111" s="15" t="s">
-        <v>531</v>
-      </c>
-      <c r="D111" s="7" t="s">
-        <v>354</v>
+        <v>533</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>348</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
       <c r="F111" s="24"/>
       <c r="G111" s="24"/>
       <c r="H111" s="24"/>
     </row>
     <row r="112">
-      <c r="C112" s="26" t="s">
-        <v>532</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>382</v>
+      <c r="C112" s="15" t="s">
+        <v>534</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>354</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>383</v>
+        <v>355</v>
       </c>
       <c r="F112" s="24"/>
       <c r="G112" s="24"/>
       <c r="H112" s="24"/>
     </row>
     <row r="113">
-      <c r="C113" s="15" t="s">
-        <v>533</v>
+      <c r="C113" s="26" t="s">
+        <v>535</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="F113" s="24"/>
       <c r="G113" s="24"/>
       <c r="H113" s="24"/>
     </row>
     <row r="114">
-      <c r="B114" s="15" t="s">
-        <v>451</v>
-      </c>
       <c r="C114" s="15" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>345</v>
+        <v>378</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>346</v>
+        <v>379</v>
       </c>
       <c r="F114" s="24"/>
       <c r="G114" s="24"/>
       <c r="H114" s="24"/>
     </row>
     <row r="115">
+      <c r="B115" s="15" t="s">
+        <v>454</v>
+      </c>
       <c r="C115" s="15" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>406</v>
+        <v>345</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>407</v>
+        <v>346</v>
       </c>
       <c r="F115" s="24"/>
       <c r="G115" s="24"/>
@@ -7202,13 +7301,13 @@
     </row>
     <row r="116">
       <c r="C116" s="15" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>400</v>
+        <v>406</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>401</v>
+        <v>407</v>
       </c>
       <c r="F116" s="24"/>
       <c r="G116" s="24"/>
@@ -7216,13 +7315,13 @@
     </row>
     <row r="117">
       <c r="C117" s="15" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F117" s="24"/>
       <c r="G117" s="24"/>
@@ -7230,13 +7329,13 @@
     </row>
     <row r="118">
       <c r="C118" s="15" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>358</v>
+        <v>402</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>359</v>
+        <v>403</v>
       </c>
       <c r="F118" s="24"/>
       <c r="G118" s="24"/>
@@ -7244,13 +7343,13 @@
     </row>
     <row r="119">
       <c r="C119" s="15" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="F119" s="24"/>
       <c r="G119" s="24"/>
@@ -7258,13 +7357,13 @@
     </row>
     <row r="120">
       <c r="C120" s="15" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F120" s="24"/>
       <c r="G120" s="24"/>
@@ -7272,13 +7371,13 @@
     </row>
     <row r="121">
       <c r="C121" s="15" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F121" s="24"/>
       <c r="G121" s="24"/>
@@ -7286,13 +7385,13 @@
     </row>
     <row r="122">
       <c r="C122" s="15" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="F122" s="24"/>
       <c r="G122" s="24"/>
@@ -7300,13 +7399,13 @@
     </row>
     <row r="123">
       <c r="C123" s="15" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="F123" s="24"/>
       <c r="G123" s="24"/>
@@ -7314,13 +7413,13 @@
     </row>
     <row r="124">
       <c r="C124" s="15" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="E124" s="3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="F124" s="24"/>
       <c r="G124" s="24"/>
@@ -7328,27 +7427,27 @@
     </row>
     <row r="125">
       <c r="C125" s="15" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="E125" s="3" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="F125" s="24"/>
       <c r="G125" s="24"/>
       <c r="H125" s="24"/>
     </row>
     <row r="126">
-      <c r="C126" s="21" t="s">
-        <v>546</v>
+      <c r="C126" s="15" t="s">
+        <v>548</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="E126" s="3" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="F126" s="24"/>
       <c r="G126" s="24"/>
@@ -7356,98 +7455,98 @@
     </row>
     <row r="127">
       <c r="C127" s="21" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>282</v>
+        <v>394</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>283</v>
+        <v>395</v>
       </c>
       <c r="F127" s="24"/>
       <c r="G127" s="24"/>
       <c r="H127" s="24"/>
     </row>
     <row r="128">
-      <c r="A128" s="21" t="s">
-        <v>548</v>
-      </c>
-      <c r="B128" s="21" t="s">
-        <v>413</v>
-      </c>
       <c r="C128" s="21" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>296</v>
+        <v>283</v>
       </c>
       <c r="F128" s="24"/>
       <c r="G128" s="24"/>
       <c r="H128" s="24"/>
     </row>
     <row r="129">
+      <c r="A129" s="21" t="s">
+        <v>551</v>
+      </c>
       <c r="B129" s="21" t="s">
-        <v>451</v>
+        <v>413</v>
       </c>
       <c r="C129" s="21" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F129" s="24"/>
       <c r="G129" s="24"/>
       <c r="H129" s="24"/>
     </row>
     <row r="130">
+      <c r="B130" s="21" t="s">
+        <v>454</v>
+      </c>
       <c r="C130" s="21" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="F130" s="24"/>
       <c r="G130" s="24"/>
       <c r="H130" s="24"/>
     </row>
     <row r="131">
-      <c r="A131" s="21" t="s">
-        <v>552</v>
-      </c>
-      <c r="B131" s="21" t="s">
-        <v>464</v>
-      </c>
       <c r="C131" s="21" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>84</v>
+        <v>298</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>226</v>
+        <v>299</v>
       </c>
       <c r="F131" s="24"/>
       <c r="G131" s="24"/>
       <c r="H131" s="24"/>
     </row>
     <row r="132">
+      <c r="A132" s="21" t="s">
+        <v>555</v>
+      </c>
+      <c r="B132" s="21" t="s">
+        <v>467</v>
+      </c>
       <c r="C132" s="21" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>97</v>
+        <v>226</v>
       </c>
       <c r="F132" s="24"/>
       <c r="G132" s="24"/>
@@ -7455,58 +7554,58 @@
     </row>
     <row r="133">
       <c r="C133" s="21" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>556</v>
+        <v>97</v>
       </c>
       <c r="F133" s="24"/>
       <c r="G133" s="24"/>
       <c r="H133" s="24"/>
     </row>
     <row r="134">
-      <c r="C134" s="8" t="s">
-        <v>557</v>
+      <c r="C134" s="21" t="s">
+        <v>558</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>233</v>
+        <v>93</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>234</v>
+        <v>559</v>
       </c>
       <c r="F134" s="24"/>
       <c r="G134" s="24"/>
       <c r="H134" s="24"/>
     </row>
     <row r="135">
-      <c r="B135" s="21" t="s">
-        <v>413</v>
-      </c>
       <c r="C135" s="8" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="F135" s="24"/>
       <c r="G135" s="24"/>
       <c r="H135" s="24"/>
     </row>
     <row r="136">
+      <c r="B136" s="21" t="s">
+        <v>413</v>
+      </c>
       <c r="C136" s="8" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>398</v>
+        <v>257</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>399</v>
+        <v>231</v>
       </c>
       <c r="F136" s="24"/>
       <c r="G136" s="24"/>
@@ -7514,13 +7613,13 @@
     </row>
     <row r="137">
       <c r="C137" s="8" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>230</v>
+        <v>398</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>87</v>
+        <v>399</v>
       </c>
       <c r="F137" s="24"/>
       <c r="G137" s="24"/>
@@ -7528,13 +7627,13 @@
     </row>
     <row r="138">
       <c r="C138" s="8" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>88</v>
+        <v>230</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F138" s="24"/>
       <c r="G138" s="24"/>
@@ -7542,13 +7641,13 @@
     </row>
     <row r="139">
       <c r="C139" s="8" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>235</v>
+        <v>88</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>236</v>
+        <v>89</v>
       </c>
       <c r="F139" s="24"/>
       <c r="G139" s="24"/>
@@ -7556,44 +7655,44 @@
     </row>
     <row r="140">
       <c r="C140" s="8" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="F140" s="24"/>
       <c r="G140" s="24"/>
       <c r="H140" s="24"/>
     </row>
     <row r="141">
-      <c r="B141" s="21" t="s">
-        <v>451</v>
-      </c>
-      <c r="C141" s="21" t="s">
-        <v>564</v>
+      <c r="C141" s="8" t="s">
+        <v>566</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="F141" s="24"/>
       <c r="G141" s="24"/>
       <c r="H141" s="24"/>
     </row>
     <row r="142">
+      <c r="B142" s="21" t="s">
+        <v>454</v>
+      </c>
       <c r="C142" s="21" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>274</v>
+        <v>240</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>275</v>
+        <v>241</v>
       </c>
       <c r="F142" s="24"/>
       <c r="G142" s="24"/>
@@ -7601,13 +7700,13 @@
     </row>
     <row r="143">
       <c r="C143" s="21" t="s">
-        <v>566</v>
-      </c>
-      <c r="D143" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="E143" s="9" t="s">
-        <v>264</v>
+        <v>568</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>275</v>
       </c>
       <c r="F143" s="24"/>
       <c r="G143" s="24"/>
@@ -7615,13 +7714,13 @@
     </row>
     <row r="144">
       <c r="C144" s="21" t="s">
-        <v>567</v>
-      </c>
-      <c r="D144" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="E144" s="3" t="s">
-        <v>228</v>
+        <v>569</v>
+      </c>
+      <c r="D144" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E144" s="9" t="s">
+        <v>264</v>
       </c>
       <c r="F144" s="24"/>
       <c r="G144" s="24"/>
@@ -7629,106 +7728,276 @@
     </row>
     <row r="145">
       <c r="C145" s="21" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>256</v>
+        <v>227</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>256</v>
+        <v>228</v>
       </c>
       <c r="F145" s="24"/>
       <c r="G145" s="24"/>
       <c r="H145" s="24"/>
     </row>
     <row r="146">
-      <c r="B146" s="21" t="s">
-        <v>445</v>
-      </c>
-      <c r="C146" s="8" t="s">
-        <v>569</v>
+      <c r="C146" s="21" t="s">
+        <v>571</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>570</v>
+        <v>256</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="F146" s="24"/>
       <c r="G146" s="24"/>
       <c r="H146" s="24"/>
     </row>
     <row r="147">
-      <c r="C147" s="8" t="s">
-        <v>571</v>
+      <c r="C147" s="21" t="s">
+        <v>572</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>252</v>
+        <v>573</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>253</v>
+        <v>574</v>
       </c>
       <c r="F147" s="24"/>
       <c r="G147" s="24"/>
       <c r="H147" s="24"/>
     </row>
     <row r="148">
+      <c r="B148" s="21" t="s">
+        <v>448</v>
+      </c>
       <c r="C148" s="8" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>259</v>
+        <v>576</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>260</v>
+        <v>577</v>
       </c>
       <c r="F148" s="24"/>
       <c r="G148" s="24"/>
       <c r="H148" s="24"/>
     </row>
     <row r="149">
-      <c r="A149" s="21"/>
-      <c r="B149" s="21"/>
-      <c r="C149" s="24"/>
-      <c r="D149" s="3"/>
-      <c r="E149" s="3"/>
+      <c r="C149" s="8" t="s">
+        <v>578</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>253</v>
+      </c>
       <c r="F149" s="24"/>
       <c r="G149" s="24"/>
       <c r="H149" s="24"/>
     </row>
+    <row r="150">
+      <c r="C150" s="8" t="s">
+        <v>580</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="F150" s="24"/>
+      <c r="G150" s="24"/>
+      <c r="H150" s="24"/>
+    </row>
+    <row r="151">
+      <c r="A151" s="21" t="s">
+        <v>581</v>
+      </c>
+      <c r="B151" s="21" t="s">
+        <v>582</v>
+      </c>
+      <c r="C151" s="21" t="s">
+        <v>583</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="F151" s="24"/>
+      <c r="G151" s="24"/>
+      <c r="H151" s="24"/>
+    </row>
+    <row r="152">
+      <c r="C152" s="21" t="s">
+        <v>586</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="F152" s="24"/>
+      <c r="G152" s="24"/>
+      <c r="H152" s="24"/>
+    </row>
+    <row r="153">
+      <c r="C153" s="21" t="s">
+        <v>589</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="F153" s="24"/>
+      <c r="G153" s="24"/>
+      <c r="H153" s="24"/>
+    </row>
+    <row r="154">
+      <c r="C154" s="21" t="s">
+        <v>592</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="F154" s="24"/>
+      <c r="G154" s="24"/>
+      <c r="H154" s="24"/>
+    </row>
+    <row r="155">
+      <c r="C155" s="21" t="s">
+        <v>595</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="F155" s="24"/>
+      <c r="G155" s="24"/>
+      <c r="H155" s="24"/>
+    </row>
+    <row r="156">
+      <c r="C156" s="21" t="s">
+        <v>598</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>599</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>600</v>
+      </c>
+      <c r="F156" s="24"/>
+      <c r="G156" s="24"/>
+      <c r="H156" s="24"/>
+    </row>
+    <row r="157">
+      <c r="C157" s="21" t="s">
+        <v>601</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="F157" s="24"/>
+      <c r="G157" s="24"/>
+      <c r="H157" s="24"/>
+    </row>
+    <row r="158">
+      <c r="C158" s="21" t="s">
+        <v>604</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="F158" s="24"/>
+      <c r="G158" s="24"/>
+      <c r="H158" s="24"/>
+    </row>
+    <row r="159">
+      <c r="B159" s="21" t="s">
+        <v>448</v>
+      </c>
+      <c r="C159" s="21" t="s">
+        <v>607</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>608</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="F159" s="24"/>
+      <c r="G159" s="24"/>
+      <c r="H159" s="24"/>
+    </row>
+    <row r="160">
+      <c r="C160" s="21" t="s">
+        <v>610</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>612</v>
+      </c>
+      <c r="F160" s="24"/>
+      <c r="G160" s="24"/>
+      <c r="H160" s="24"/>
+    </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="B86:B98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B57"/>
-    <mergeCell ref="A58:A65"/>
-    <mergeCell ref="B58:B63"/>
-    <mergeCell ref="A66:A76"/>
-    <mergeCell ref="B66:B72"/>
-    <mergeCell ref="A82:A100"/>
+  <mergeCells count="34">
+    <mergeCell ref="B132:B135"/>
+    <mergeCell ref="B136:B141"/>
+    <mergeCell ref="A102:A128"/>
+    <mergeCell ref="B102:B110"/>
+    <mergeCell ref="B111:B114"/>
+    <mergeCell ref="B115:B128"/>
+    <mergeCell ref="A129:A131"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="A132:A150"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
-    <mergeCell ref="A4:A38"/>
-    <mergeCell ref="B4:B34"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="A39:A57"/>
-    <mergeCell ref="B39:B48"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="A77:A81"/>
-    <mergeCell ref="B77:B80"/>
-    <mergeCell ref="B135:B140"/>
-    <mergeCell ref="B146:B148"/>
-    <mergeCell ref="B131:B134"/>
-    <mergeCell ref="B141:B145"/>
-    <mergeCell ref="B101:B109"/>
-    <mergeCell ref="A128:A130"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="B110:B113"/>
-    <mergeCell ref="A101:A127"/>
-    <mergeCell ref="B114:B127"/>
-    <mergeCell ref="A131:A148"/>
+    <mergeCell ref="A4:A39"/>
+    <mergeCell ref="B4:B35"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="A40:A58"/>
+    <mergeCell ref="B40:B49"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="B78:B81"/>
+    <mergeCell ref="A78:A82"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B87:B99"/>
+    <mergeCell ref="B100:B101"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B52:B58"/>
+    <mergeCell ref="A59:A66"/>
+    <mergeCell ref="B59:B64"/>
+    <mergeCell ref="A67:A77"/>
+    <mergeCell ref="B67:B73"/>
+    <mergeCell ref="A83:A101"/>
+    <mergeCell ref="B142:B147"/>
+    <mergeCell ref="B148:B150"/>
+    <mergeCell ref="B151:B158"/>
+    <mergeCell ref="B159:B160"/>
+    <mergeCell ref="A151:A160"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: i18n 최신화 (#146)
</commit_message>
<xml_diff>
--- a/scripts/i18n.xlsx
+++ b/scripts/i18n.xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="668">
   <si>
     <t xml:space="preserve">페이지는 [피그마] PFPlay GUI 설계서 합본의 페이지 이름입니다. </t>
   </si>
@@ -1597,15 +1597,9 @@
     <t>auth.para.auth_changed</t>
   </si>
   <si>
-    <t>Permissions have been changed!</t>
-  </si>
-  <si>
     <t>auth.para.auth_quota_exceeded</t>
   </si>
   <si>
-    <t>The limit for this permission has been exceeded</t>
-  </si>
-  <si>
     <t>auth.para.no_change_authority</t>
   </si>
   <si>
@@ -1819,34 +1813,49 @@
     <t>party.para.auto_close_30days</t>
   </si>
   <si>
-    <t>현재 파티룸을 정말로 폐쇄하시겠어요? 모든 데이터는 저장되지 않습니다.</t>
+    <t>If there is no DJing for 30 days, the party room will automatically close</t>
   </si>
   <si>
     <t>party.para.existing_party</t>
   </si>
   <si>
+    <t>It's already an existing party name</t>
+  </si>
+  <si>
+    <t>party.para.more_than_3m</t>
+  </si>
+  <si>
+    <t>Available for more than 3 minutes</t>
+  </si>
+  <si>
+    <t>party.para.stop_editing</t>
+  </si>
+  <si>
+    <t>지금까지 작성한 내용은 저장되지 않아요.\n수정을 그만하시겠어요?</t>
+  </si>
+  <si>
+    <t>The content written so far is not saved.\nWould you like to stop editing?</t>
+  </si>
+  <si>
+    <t>party.para.copy_completed</t>
+  </si>
+  <si>
+    <t>party.para.close_party</t>
+  </si>
+  <si>
+    <t>현재 파티룸을 정말로 폐쇄하시겠어요?\n모든 데이터는 저장되지 않습니다.</t>
+  </si>
+  <si>
+    <t>Are you sure you want to close the current party room?\nAll data will not be saved.</t>
+  </si>
+  <si>
+    <t>party.para.enter_confirm</t>
+  </si>
+  <si>
     <t>'확인했습니다' 입력</t>
   </si>
   <si>
-    <t>party.para.more_than_3m</t>
-  </si>
-  <si>
-    <t>You will no longer see this user's chat in this room (only applies to you)</t>
-  </si>
-  <si>
-    <t>party.para.stop_editing</t>
-  </si>
-  <si>
-    <t>party.para.copy_completed</t>
-  </si>
-  <si>
-    <t>변경 내용이 저장되지 않아요. 파티룸으로 나가시겠어요?</t>
-  </si>
-  <si>
-    <t>party.para.close_party</t>
-  </si>
-  <si>
-    <t>party.para.enter_confirm</t>
+    <t>Enter 'Confirmed'</t>
   </si>
   <si>
     <t>party.para.no_longer_see_chat</t>
@@ -1858,15 +1867,18 @@
     <t>party.para.leave_party_confirm</t>
   </si>
   <si>
+    <t>변경 내용이 저장되지 않아요.\n파티룸으로 나가시겠어요?</t>
+  </si>
+  <si>
+    <t>Your changes won't be saved.\nAre you sure you want to leave the party room?</t>
+  </si>
+  <si>
     <t>party.para.close</t>
   </si>
   <si>
     <t>party.para.enter_confirm_phrase</t>
   </si>
   <si>
-    <t>Please enter the confirmation phrase</t>
-  </si>
-  <si>
     <t>party.btn.share_twitter</t>
   </si>
   <si>
@@ -1936,13 +1948,16 @@
     <t>현재 디제잉 인원이 없어요\n파티의 흥을 책임질 DJ가 되어보세요!</t>
   </si>
   <si>
-    <t>There are no DJs currently.\nBecome a DJ and keep the party going!</t>
-  </si>
-  <si>
-    <t>dj.para.create_playlist_first</t>
-  </si>
-  <si>
-    <t>Please create a playlist to register</t>
+    <t>No one is djing now.\nWhy not become the DJ and make some noise!</t>
+  </si>
+  <si>
+    <t>dj.para.create_playlist_song</t>
+  </si>
+  <si>
+    <t>대기 등록을 위해 최소 1곡이 담긴 플레이리스트가 필요해요</t>
+  </si>
+  <si>
+    <t>Before you join the queue, please create a playlist with at least one song.</t>
   </si>
   <si>
     <t>dj.para.cancel_dj_queue</t>
@@ -1951,9 +1966,6 @@
     <t>dj.para.cancel_dj_queue_confirm</t>
   </si>
   <si>
-    <t>Are you sure you want to cancel your DJ queue registration?</t>
-  </si>
-  <si>
     <t>dj.para.lock_dj_queue</t>
   </si>
   <si>
@@ -2017,7 +2029,7 @@
     <t>ed.para.noti_deleted</t>
   </si>
   <si>
-    <t>Existing notices will be deleted upon registration!</t>
+    <t>When you add a new announcement, the old one will be removed!</t>
   </si>
   <si>
     <t>플레이 리스트 (Playlist)</t>
@@ -2074,11 +2086,10 @@
     <t>playlist.para.delete_duplicated_list_confirm</t>
   </si>
   <si>
-    <t>$1'에 이미 존재하는 곡입니다! 
-중복곡은 삭제하고 다시 담을까요?</t>
-  </si>
-  <si>
-    <t>$1' already has this song! Shall we delete the duplicate song and put it back?</t>
+    <t>'$1'에 이미 존재하는 곡입니다!\n중복곡은 삭제하고 다시 담을까요?</t>
+  </si>
+  <si>
+    <t>'$1' already has this song!\nShould we remove the duplicate and add it again?</t>
   </si>
   <si>
     <t>playlist.para.no_list_yet</t>
@@ -2119,9 +2130,6 @@
   </si>
   <si>
     <t>playlist.ec.up_to_100_songs</t>
-  </si>
-  <si>
-    <t>You can only add up to 100 songs per playlist</t>
   </si>
   <si>
     <t>파티룸 입장(Partyroom)</t>
@@ -2194,7 +2202,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2229,6 +2237,15 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF444746"/>
+      <name val="&quot;Google Sans&quot;"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Roboto"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2256,7 +2273,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2329,9 +2346,22 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="center"/>
     </xf>
-    <xf quotePrefix="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf quotePrefix="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -5858,9 +5888,9 @@
     <col customWidth="1" min="1" max="1" width="20.13"/>
     <col customWidth="1" min="2" max="2" width="23.0"/>
     <col customWidth="1" min="3" max="3" width="32.63"/>
-    <col customWidth="1" min="4" max="4" width="46.13"/>
+    <col customWidth="1" min="4" max="4" width="48.75"/>
     <col customWidth="1" min="5" max="7" width="43.75"/>
-    <col customWidth="1" min="8" max="8" width="22.0"/>
+    <col customWidth="1" min="8" max="13" width="22.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5871,6 +5901,11 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
@@ -5880,6 +5915,11 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
@@ -5906,6 +5946,11 @@
       <c r="H3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="16" t="s">
@@ -5926,6 +5971,11 @@
       <c r="F4" s="17"/>
       <c r="G4" s="18"/>
       <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
     </row>
     <row r="5">
       <c r="C5" s="16" t="s">
@@ -5940,6 +5990,11 @@
       <c r="F5" s="17"/>
       <c r="G5" s="18"/>
       <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
     </row>
     <row r="6">
       <c r="C6" s="16" t="s">
@@ -5954,6 +6009,11 @@
       <c r="F6" s="17"/>
       <c r="G6" s="18"/>
       <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
     </row>
     <row r="7">
       <c r="C7" s="16" t="s">
@@ -5968,6 +6028,11 @@
       <c r="F7" s="17"/>
       <c r="G7" s="18"/>
       <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
     </row>
     <row r="8">
       <c r="C8" s="16" t="s">
@@ -5982,6 +6047,11 @@
       <c r="F8" s="17"/>
       <c r="G8" s="18"/>
       <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
     </row>
     <row r="9">
       <c r="C9" s="16" t="s">
@@ -5996,6 +6066,11 @@
       <c r="F9" s="17"/>
       <c r="G9" s="18"/>
       <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
     </row>
     <row r="10">
       <c r="C10" s="16" t="s">
@@ -6010,6 +6085,11 @@
       <c r="F10" s="17"/>
       <c r="G10" s="18"/>
       <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
     </row>
     <row r="11">
       <c r="C11" s="16" t="s">
@@ -6024,6 +6104,11 @@
       <c r="F11" s="17"/>
       <c r="G11" s="18"/>
       <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
     </row>
     <row r="12">
       <c r="C12" s="16" t="s">
@@ -6038,6 +6123,11 @@
       <c r="F12" s="17"/>
       <c r="G12" s="18"/>
       <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="17"/>
+      <c r="L12" s="17"/>
+      <c r="M12" s="17"/>
     </row>
     <row r="13">
       <c r="C13" s="16" t="s">
@@ -6052,6 +6142,11 @@
       <c r="F13" s="17"/>
       <c r="G13" s="18"/>
       <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="17"/>
+      <c r="L13" s="17"/>
+      <c r="M13" s="17"/>
     </row>
     <row r="14">
       <c r="C14" s="16" t="s">
@@ -6066,6 +6161,11 @@
       <c r="F14" s="17"/>
       <c r="G14" s="18"/>
       <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
     </row>
     <row r="15">
       <c r="C15" s="16" t="s">
@@ -6080,6 +6180,11 @@
       <c r="F15" s="17"/>
       <c r="G15" s="18"/>
       <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17"/>
+      <c r="M15" s="17"/>
     </row>
     <row r="16">
       <c r="C16" s="16" t="s">
@@ -6094,6 +6199,11 @@
       <c r="F16" s="17"/>
       <c r="G16" s="18"/>
       <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
     </row>
     <row r="17">
       <c r="C17" s="16" t="s">
@@ -6108,6 +6218,11 @@
       <c r="F17" s="17"/>
       <c r="G17" s="18"/>
       <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
     </row>
     <row r="18">
       <c r="C18" s="16" t="s">
@@ -6122,6 +6237,11 @@
       <c r="F18" s="17"/>
       <c r="G18" s="18"/>
       <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
     </row>
     <row r="19">
       <c r="C19" s="16" t="s">
@@ -6136,6 +6256,11 @@
       <c r="F19" s="17"/>
       <c r="G19" s="18"/>
       <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="17"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
     </row>
     <row r="20">
       <c r="C20" s="19" t="s">
@@ -6150,6 +6275,11 @@
       <c r="F20" s="17"/>
       <c r="G20" s="18"/>
       <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
     </row>
     <row r="21">
       <c r="C21" s="16" t="s">
@@ -6164,6 +6294,11 @@
       <c r="F21" s="17"/>
       <c r="G21" s="18"/>
       <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
     </row>
     <row r="22">
       <c r="C22" s="16" t="s">
@@ -6178,6 +6313,11 @@
       <c r="F22" s="17"/>
       <c r="G22" s="18"/>
       <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
     </row>
     <row r="23">
       <c r="C23" s="20" t="s">
@@ -6192,6 +6332,11 @@
       <c r="F23" s="17"/>
       <c r="G23" s="18"/>
       <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
     </row>
     <row r="24">
       <c r="C24" s="20" t="s">
@@ -6206,6 +6351,11 @@
       <c r="F24" s="17"/>
       <c r="G24" s="18"/>
       <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
     </row>
     <row r="25">
       <c r="C25" s="20" t="s">
@@ -6220,6 +6370,11 @@
       <c r="F25" s="17"/>
       <c r="G25" s="18"/>
       <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
     </row>
     <row r="26">
       <c r="C26" s="20" t="s">
@@ -6234,6 +6389,11 @@
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
       <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
     </row>
     <row r="27">
       <c r="C27" s="20" t="s">
@@ -6248,6 +6408,11 @@
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
       <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="17"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
     </row>
     <row r="28">
       <c r="C28" s="20" t="s">
@@ -6262,6 +6427,11 @@
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
       <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+      <c r="J28" s="17"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
     </row>
     <row r="29">
       <c r="C29" s="16" t="s">
@@ -6276,6 +6446,11 @@
       <c r="F29" s="17"/>
       <c r="G29" s="18"/>
       <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
     </row>
     <row r="30">
       <c r="C30" s="16" t="s">
@@ -6290,6 +6465,11 @@
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
       <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
     </row>
     <row r="31">
       <c r="C31" s="19" t="s">
@@ -6304,6 +6484,11 @@
       <c r="F31" s="17"/>
       <c r="G31" s="18"/>
       <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
     </row>
     <row r="32">
       <c r="C32" s="19" t="s">
@@ -6318,6 +6503,11 @@
       <c r="F32" s="17"/>
       <c r="G32" s="18"/>
       <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
     </row>
     <row r="33">
       <c r="C33" s="19" t="s">
@@ -6332,6 +6522,11 @@
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
       <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17"/>
+      <c r="M33" s="17"/>
     </row>
     <row r="34">
       <c r="C34" s="19" t="s">
@@ -6346,6 +6541,11 @@
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
       <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
     </row>
     <row r="35">
       <c r="C35" s="19" t="s">
@@ -6360,6 +6560,11 @@
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
       <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
+      <c r="M35" s="17"/>
     </row>
     <row r="36">
       <c r="B36" s="16" t="s">
@@ -6377,6 +6582,11 @@
       <c r="F36" s="17"/>
       <c r="G36" s="18"/>
       <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
     </row>
     <row r="37">
       <c r="C37" s="7" t="s">
@@ -6391,6 +6601,11 @@
       <c r="F37" s="17"/>
       <c r="G37" s="18"/>
       <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="17"/>
+      <c r="M37" s="17"/>
     </row>
     <row r="38">
       <c r="C38" s="7" t="s">
@@ -6405,6 +6620,11 @@
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
       <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
     </row>
     <row r="39">
       <c r="C39" s="7" t="s">
@@ -6419,6 +6639,11 @@
       <c r="F39" s="17"/>
       <c r="G39" s="18"/>
       <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="17"/>
+      <c r="M39" s="17"/>
     </row>
     <row r="40">
       <c r="A40" s="16"/>
@@ -6435,6 +6660,11 @@
       <c r="F40" s="17"/>
       <c r="G40" s="18"/>
       <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="17"/>
     </row>
     <row r="41">
       <c r="A41" s="16"/>
@@ -6451,6 +6681,11 @@
       <c r="F41" s="17"/>
       <c r="G41" s="18"/>
       <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="17"/>
+      <c r="K41" s="17"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
     </row>
     <row r="42">
       <c r="A42" s="16"/>
@@ -6467,6 +6702,11 @@
       <c r="F42" s="17"/>
       <c r="G42" s="18"/>
       <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
     </row>
     <row r="43">
       <c r="A43" s="16" t="s">
@@ -6487,6 +6727,11 @@
       <c r="F43" s="17"/>
       <c r="G43" s="18"/>
       <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+      <c r="K43" s="17"/>
+      <c r="L43" s="17"/>
+      <c r="M43" s="17"/>
     </row>
     <row r="44">
       <c r="C44" s="16" t="s">
@@ -6501,6 +6746,11 @@
       <c r="F44" s="17"/>
       <c r="G44" s="18"/>
       <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+      <c r="K44" s="17"/>
+      <c r="L44" s="17"/>
+      <c r="M44" s="17"/>
     </row>
     <row r="45">
       <c r="C45" s="16" t="s">
@@ -6515,6 +6765,11 @@
       <c r="F45" s="17"/>
       <c r="G45" s="18"/>
       <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="17"/>
+      <c r="M45" s="17"/>
     </row>
     <row r="46">
       <c r="C46" s="19" t="s">
@@ -6529,6 +6784,11 @@
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
       <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="17"/>
+      <c r="M46" s="17"/>
     </row>
     <row r="47">
       <c r="C47" s="19" t="s">
@@ -6543,6 +6803,11 @@
       <c r="F47" s="17"/>
       <c r="G47" s="18"/>
       <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
     </row>
     <row r="48">
       <c r="C48" s="19" t="s">
@@ -6557,6 +6822,11 @@
       <c r="F48" s="17"/>
       <c r="G48" s="18"/>
       <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="17"/>
+      <c r="M48" s="17"/>
     </row>
     <row r="49">
       <c r="C49" s="19" t="s">
@@ -6571,6 +6841,11 @@
       <c r="F49" s="17"/>
       <c r="G49" s="18"/>
       <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="17"/>
+      <c r="M49" s="17"/>
     </row>
     <row r="50">
       <c r="C50" s="19" t="s">
@@ -6579,30 +6854,40 @@
       <c r="D50" s="8" t="s">
         <v>303</v>
       </c>
-      <c r="E50" s="8" t="s">
-        <v>468</v>
+      <c r="E50" s="3" t="s">
+        <v>304</v>
       </c>
       <c r="F50" s="17"/>
       <c r="G50" s="18"/>
       <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
     </row>
     <row r="51">
       <c r="C51" s="19" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>306</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>470</v>
+        <v>307</v>
       </c>
       <c r="F51" s="17"/>
       <c r="G51" s="18"/>
       <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+      <c r="J51" s="17"/>
+      <c r="K51" s="17"/>
+      <c r="L51" s="17"/>
+      <c r="M51" s="17"/>
     </row>
     <row r="52">
       <c r="C52" s="19" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="D52" s="8" t="s">
         <v>309</v>
@@ -6613,13 +6898,18 @@
       <c r="F52" s="17"/>
       <c r="G52" s="18"/>
       <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
     </row>
     <row r="53">
       <c r="B53" s="19" t="s">
         <v>395</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D53" s="8" t="s">
         <v>230</v>
@@ -6630,10 +6920,15 @@
       <c r="F53" s="17"/>
       <c r="G53" s="18"/>
       <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="17"/>
+      <c r="K53" s="17"/>
+      <c r="L53" s="17"/>
+      <c r="M53" s="17"/>
     </row>
     <row r="54">
       <c r="C54" s="19" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="D54" s="8" t="s">
         <v>27</v>
@@ -6644,27 +6939,37 @@
       <c r="F54" s="17"/>
       <c r="G54" s="18"/>
       <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+      <c r="J54" s="17"/>
+      <c r="K54" s="17"/>
+      <c r="L54" s="17"/>
+      <c r="M54" s="17"/>
     </row>
     <row r="55">
       <c r="B55" s="19" t="s">
+        <v>472</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>473</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>474</v>
       </c>
-      <c r="C55" s="19" t="s">
+      <c r="E55" s="8" t="s">
         <v>475</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>476</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>477</v>
       </c>
       <c r="F55" s="17"/>
       <c r="G55" s="18"/>
       <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+      <c r="J55" s="17"/>
+      <c r="K55" s="17"/>
+      <c r="L55" s="17"/>
+      <c r="M55" s="17"/>
     </row>
     <row r="56">
       <c r="C56" s="19" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>296</v>
@@ -6675,10 +6980,15 @@
       <c r="F56" s="17"/>
       <c r="G56" s="18"/>
       <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="17"/>
+      <c r="L56" s="17"/>
+      <c r="M56" s="17"/>
     </row>
     <row r="57">
       <c r="C57" s="19" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="D57" s="8" t="s">
         <v>298</v>
@@ -6689,10 +6999,15 @@
       <c r="F57" s="17"/>
       <c r="G57" s="18"/>
       <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="17"/>
+      <c r="K57" s="17"/>
+      <c r="L57" s="17"/>
+      <c r="M57" s="17"/>
     </row>
     <row r="58">
       <c r="C58" s="19" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D58" s="8" t="s">
         <v>299</v>
@@ -6703,10 +7018,15 @@
       <c r="F58" s="17"/>
       <c r="G58" s="18"/>
       <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+      <c r="J58" s="17"/>
+      <c r="K58" s="17"/>
+      <c r="L58" s="17"/>
+      <c r="M58" s="17"/>
     </row>
     <row r="59">
       <c r="C59" s="19" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="D59" s="8" t="s">
         <v>300</v>
@@ -6717,10 +7037,15 @@
       <c r="F59" s="17"/>
       <c r="G59" s="18"/>
       <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="17"/>
+      <c r="L59" s="17"/>
+      <c r="M59" s="17"/>
     </row>
     <row r="60">
       <c r="C60" s="19" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D60" s="8" t="s">
         <v>301</v>
@@ -6731,10 +7056,15 @@
       <c r="F60" s="17"/>
       <c r="G60" s="18"/>
       <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
+      <c r="J60" s="17"/>
+      <c r="K60" s="17"/>
+      <c r="L60" s="17"/>
+      <c r="M60" s="17"/>
     </row>
     <row r="61">
       <c r="C61" s="19" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D61" s="8" t="s">
         <v>177</v>
@@ -6745,16 +7075,21 @@
       <c r="F61" s="17"/>
       <c r="G61" s="18"/>
       <c r="H61" s="17"/>
+      <c r="I61" s="17"/>
+      <c r="J61" s="17"/>
+      <c r="K61" s="17"/>
+      <c r="L61" s="17"/>
+      <c r="M61" s="17"/>
     </row>
     <row r="62">
       <c r="A62" s="19" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B62" s="19" t="s">
         <v>395</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>11</v>
@@ -6765,10 +7100,15 @@
       <c r="F62" s="17"/>
       <c r="G62" s="18"/>
       <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17"/>
+      <c r="K62" s="17"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="17"/>
     </row>
     <row r="63">
       <c r="C63" s="19" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="D63" s="3" t="s">
         <v>14</v>
@@ -6779,10 +7119,15 @@
       <c r="F63" s="17"/>
       <c r="G63" s="18"/>
       <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
     </row>
     <row r="64">
       <c r="C64" s="19" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="D64" s="8" t="s">
         <v>15</v>
@@ -6793,10 +7138,15 @@
       <c r="F64" s="17"/>
       <c r="G64" s="18"/>
       <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
     </row>
     <row r="65">
       <c r="C65" s="19" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D65" s="8" t="s">
         <v>18</v>
@@ -6807,10 +7157,15 @@
       <c r="F65" s="17"/>
       <c r="G65" s="18"/>
       <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
+      <c r="J65" s="17"/>
+      <c r="K65" s="17"/>
+      <c r="L65" s="17"/>
+      <c r="M65" s="17"/>
     </row>
     <row r="66">
       <c r="C66" s="19" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="D66" s="8" t="s">
         <v>30</v>
@@ -6821,13 +7176,18 @@
       <c r="F66" s="17"/>
       <c r="G66" s="18"/>
       <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+      <c r="J66" s="17"/>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="17"/>
     </row>
     <row r="67">
       <c r="C67" s="19" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>26</v>
@@ -6835,13 +7195,18 @@
       <c r="F67" s="17"/>
       <c r="G67" s="18"/>
       <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
     </row>
     <row r="68">
       <c r="B68" s="19" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>21</v>
@@ -6852,33 +7217,43 @@
       <c r="F68" s="17"/>
       <c r="G68" s="18"/>
       <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+      <c r="J68" s="17"/>
+      <c r="K68" s="17"/>
+      <c r="L68" s="17"/>
+      <c r="M68" s="17"/>
     </row>
     <row r="69">
       <c r="B69" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C69" s="19" t="s">
+        <v>491</v>
+      </c>
+      <c r="D69" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="E69" s="8" t="s">
         <v>493</v>
-      </c>
-      <c r="D69" s="8" t="s">
-        <v>494</v>
-      </c>
-      <c r="E69" s="8" t="s">
-        <v>495</v>
       </c>
       <c r="F69" s="17"/>
       <c r="G69" s="18"/>
       <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+      <c r="J69" s="17"/>
+      <c r="K69" s="17"/>
+      <c r="L69" s="17"/>
+      <c r="M69" s="17"/>
     </row>
     <row r="70">
       <c r="A70" s="19" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>32</v>
@@ -6889,10 +7264,15 @@
       <c r="F70" s="17"/>
       <c r="G70" s="18"/>
       <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+      <c r="J70" s="17"/>
+      <c r="K70" s="17"/>
+      <c r="L70" s="17"/>
+      <c r="M70" s="17"/>
     </row>
     <row r="71">
       <c r="C71" s="19" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>34</v>
@@ -6903,10 +7283,15 @@
       <c r="F71" s="17"/>
       <c r="G71" s="18"/>
       <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
+      <c r="J71" s="17"/>
+      <c r="K71" s="17"/>
+      <c r="L71" s="17"/>
+      <c r="M71" s="17"/>
     </row>
     <row r="72">
       <c r="C72" s="19" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>38</v>
@@ -6917,10 +7302,15 @@
       <c r="F72" s="17"/>
       <c r="G72" s="18"/>
       <c r="H72" s="17"/>
+      <c r="I72" s="17"/>
+      <c r="J72" s="17"/>
+      <c r="K72" s="17"/>
+      <c r="L72" s="17"/>
+      <c r="M72" s="17"/>
     </row>
     <row r="73">
       <c r="C73" s="19" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>46</v>
@@ -6931,10 +7321,15 @@
       <c r="F73" s="17"/>
       <c r="G73" s="18"/>
       <c r="H73" s="17"/>
+      <c r="I73" s="17"/>
+      <c r="J73" s="17"/>
+      <c r="K73" s="17"/>
+      <c r="L73" s="17"/>
+      <c r="M73" s="17"/>
     </row>
     <row r="74">
       <c r="C74" s="19" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>49</v>
@@ -6945,10 +7340,15 @@
       <c r="F74" s="17"/>
       <c r="G74" s="18"/>
       <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+      <c r="J74" s="17"/>
+      <c r="K74" s="17"/>
+      <c r="L74" s="17"/>
+      <c r="M74" s="17"/>
     </row>
     <row r="75">
       <c r="C75" s="19" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>51</v>
@@ -6959,10 +7359,15 @@
       <c r="F75" s="17"/>
       <c r="G75" s="18"/>
       <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+      <c r="J75" s="17"/>
+      <c r="K75" s="17"/>
+      <c r="L75" s="17"/>
+      <c r="M75" s="17"/>
     </row>
     <row r="76">
       <c r="C76" s="19" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>53</v>
@@ -6973,13 +7378,18 @@
       <c r="F76" s="17"/>
       <c r="G76" s="18"/>
       <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
+      <c r="J76" s="17"/>
+      <c r="K76" s="17"/>
+      <c r="L76" s="17"/>
+      <c r="M76" s="17"/>
     </row>
     <row r="77">
       <c r="B77" s="19" t="s">
         <v>436</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="D77" s="8" t="s">
         <v>57</v>
@@ -6990,13 +7400,18 @@
       <c r="F77" s="17"/>
       <c r="G77" s="18"/>
       <c r="H77" s="17"/>
+      <c r="I77" s="17"/>
+      <c r="J77" s="17"/>
+      <c r="K77" s="17"/>
+      <c r="L77" s="17"/>
+      <c r="M77" s="17"/>
     </row>
     <row r="78">
       <c r="B78" s="19" t="s">
         <v>395</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="D78" s="8" t="s">
         <v>60</v>
@@ -7007,27 +7422,37 @@
       <c r="F78" s="17"/>
       <c r="G78" s="18"/>
       <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
+      <c r="J78" s="17"/>
+      <c r="K78" s="17"/>
+      <c r="L78" s="17"/>
+      <c r="M78" s="17"/>
     </row>
     <row r="79">
       <c r="B79" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="D79" s="8" t="s">
         <v>45</v>
       </c>
       <c r="E79" s="8" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F79" s="17"/>
       <c r="G79" s="18"/>
       <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
+      <c r="J79" s="17"/>
+      <c r="K79" s="17"/>
+      <c r="L79" s="17"/>
+      <c r="M79" s="17"/>
     </row>
     <row r="80">
       <c r="C80" s="3" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="D80" s="8" t="s">
         <v>62</v>
@@ -7038,16 +7463,21 @@
       <c r="F80" s="22"/>
       <c r="G80" s="22"/>
       <c r="H80" s="22"/>
+      <c r="I80" s="22"/>
+      <c r="J80" s="22"/>
+      <c r="K80" s="22"/>
+      <c r="L80" s="22"/>
+      <c r="M80" s="22"/>
     </row>
     <row r="81">
       <c r="A81" s="19" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C81" s="19" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="D81" s="8" t="s">
         <v>74</v>
@@ -7058,10 +7488,15 @@
       <c r="F81" s="17"/>
       <c r="G81" s="18"/>
       <c r="H81" s="17"/>
+      <c r="I81" s="17"/>
+      <c r="J81" s="17"/>
+      <c r="K81" s="17"/>
+      <c r="L81" s="17"/>
+      <c r="M81" s="17"/>
     </row>
     <row r="82">
       <c r="C82" s="19" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="D82" s="8" t="s">
         <v>94</v>
@@ -7072,10 +7507,15 @@
       <c r="F82" s="17"/>
       <c r="G82" s="18"/>
       <c r="H82" s="17"/>
+      <c r="I82" s="17"/>
+      <c r="J82" s="17"/>
+      <c r="K82" s="17"/>
+      <c r="L82" s="17"/>
+      <c r="M82" s="17"/>
     </row>
     <row r="83">
       <c r="C83" s="19" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="D83" s="8" t="s">
         <v>96</v>
@@ -7086,10 +7526,15 @@
       <c r="F83" s="17"/>
       <c r="G83" s="18"/>
       <c r="H83" s="17"/>
+      <c r="I83" s="17"/>
+      <c r="J83" s="17"/>
+      <c r="K83" s="17"/>
+      <c r="L83" s="17"/>
+      <c r="M83" s="17"/>
     </row>
     <row r="84">
       <c r="C84" s="19" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="D84" s="8" t="s">
         <v>98</v>
@@ -7100,13 +7545,18 @@
       <c r="F84" s="17"/>
       <c r="G84" s="18"/>
       <c r="H84" s="17"/>
+      <c r="I84" s="17"/>
+      <c r="J84" s="17"/>
+      <c r="K84" s="17"/>
+      <c r="L84" s="17"/>
+      <c r="M84" s="17"/>
     </row>
     <row r="85">
       <c r="B85" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="D85" s="8" t="s">
         <v>75</v>
@@ -7117,16 +7567,21 @@
       <c r="F85" s="17"/>
       <c r="G85" s="18"/>
       <c r="H85" s="17"/>
+      <c r="I85" s="17"/>
+      <c r="J85" s="17"/>
+      <c r="K85" s="17"/>
+      <c r="L85" s="17"/>
+      <c r="M85" s="17"/>
     </row>
     <row r="86">
       <c r="A86" s="7" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B86" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C86" s="19" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="D86" s="8" t="s">
         <v>381</v>
@@ -7137,16 +7592,21 @@
       <c r="F86" s="17"/>
       <c r="G86" s="18"/>
       <c r="H86" s="17"/>
+      <c r="I86" s="17"/>
+      <c r="J86" s="17"/>
+      <c r="K86" s="17"/>
+      <c r="L86" s="17"/>
+      <c r="M86" s="17"/>
     </row>
     <row r="87">
       <c r="A87" s="7" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B87" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="D87" s="8" t="s">
         <v>382</v>
@@ -7157,39 +7617,49 @@
       <c r="F87" s="17"/>
       <c r="G87" s="18"/>
       <c r="H87" s="17"/>
+      <c r="I87" s="17"/>
+      <c r="J87" s="17"/>
+      <c r="K87" s="17"/>
+      <c r="L87" s="17"/>
+      <c r="M87" s="17"/>
     </row>
     <row r="88">
       <c r="A88" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B88" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C88" s="19" t="s">
+        <v>516</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="E88" s="8" t="s">
         <v>518</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="E88" s="8" t="s">
-        <v>520</v>
       </c>
       <c r="F88" s="22"/>
       <c r="G88" s="22"/>
       <c r="H88" s="22"/>
+      <c r="I88" s="22"/>
+      <c r="J88" s="22"/>
+      <c r="K88" s="22"/>
+      <c r="L88" s="22"/>
+      <c r="M88" s="22"/>
     </row>
     <row r="89">
       <c r="A89" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B89" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C89" s="19" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="E89" s="3" t="s">
         <v>159</v>
@@ -7197,16 +7667,21 @@
       <c r="F89" s="22"/>
       <c r="G89" s="22"/>
       <c r="H89" s="22"/>
+      <c r="I89" s="22"/>
+      <c r="J89" s="22"/>
+      <c r="K89" s="22"/>
+      <c r="L89" s="22"/>
+      <c r="M89" s="22"/>
     </row>
     <row r="90">
       <c r="A90" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B90" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C90" s="19" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="D90" s="3" t="s">
         <v>375</v>
@@ -7217,16 +7692,21 @@
       <c r="F90" s="22"/>
       <c r="G90" s="22"/>
       <c r="H90" s="22"/>
+      <c r="I90" s="22"/>
+      <c r="J90" s="22"/>
+      <c r="K90" s="22"/>
+      <c r="L90" s="22"/>
+      <c r="M90" s="22"/>
     </row>
     <row r="91">
       <c r="A91" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B91" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C91" s="19" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D91" s="8" t="s">
         <v>377</v>
@@ -7237,16 +7717,21 @@
       <c r="F91" s="22"/>
       <c r="G91" s="22"/>
       <c r="H91" s="22"/>
+      <c r="I91" s="22"/>
+      <c r="J91" s="22"/>
+      <c r="K91" s="22"/>
+      <c r="L91" s="22"/>
+      <c r="M91" s="22"/>
     </row>
     <row r="92">
       <c r="A92" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B92" s="19" t="s">
         <v>395</v>
       </c>
       <c r="C92" s="19" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>379</v>
@@ -7257,16 +7742,21 @@
       <c r="F92" s="22"/>
       <c r="G92" s="22"/>
       <c r="H92" s="22"/>
+      <c r="I92" s="22"/>
+      <c r="J92" s="22"/>
+      <c r="K92" s="22"/>
+      <c r="L92" s="22"/>
+      <c r="M92" s="22"/>
     </row>
     <row r="93">
       <c r="A93" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C93" s="19" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="D93" s="8" t="s">
         <v>384</v>
@@ -7277,36 +7767,46 @@
       <c r="F93" s="22"/>
       <c r="G93" s="22"/>
       <c r="H93" s="22"/>
+      <c r="I93" s="22"/>
+      <c r="J93" s="22"/>
+      <c r="K93" s="22"/>
+      <c r="L93" s="22"/>
+      <c r="M93" s="22"/>
     </row>
     <row r="94">
       <c r="A94" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B94" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C94" s="19" t="s">
+        <v>525</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>526</v>
+      </c>
+      <c r="E94" s="8" t="s">
         <v>527</v>
-      </c>
-      <c r="D94" s="8" t="s">
-        <v>528</v>
-      </c>
-      <c r="E94" s="8" t="s">
-        <v>529</v>
       </c>
       <c r="F94" s="22"/>
       <c r="G94" s="22"/>
       <c r="H94" s="22"/>
+      <c r="I94" s="22"/>
+      <c r="J94" s="22"/>
+      <c r="K94" s="22"/>
+      <c r="L94" s="22"/>
+      <c r="M94" s="22"/>
     </row>
     <row r="95">
       <c r="A95" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B95" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C95" s="19" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D95" s="8" t="s">
         <v>387</v>
@@ -7317,16 +7817,21 @@
       <c r="F95" s="22"/>
       <c r="G95" s="22"/>
       <c r="H95" s="22"/>
+      <c r="I95" s="22"/>
+      <c r="J95" s="22"/>
+      <c r="K95" s="22"/>
+      <c r="L95" s="22"/>
+      <c r="M95" s="22"/>
     </row>
     <row r="96">
       <c r="A96" s="19" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="B96" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C96" s="19" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D96" s="8" t="s">
         <v>389</v>
@@ -7337,16 +7842,21 @@
       <c r="F96" s="22"/>
       <c r="G96" s="22"/>
       <c r="H96" s="22"/>
+      <c r="I96" s="22"/>
+      <c r="J96" s="22"/>
+      <c r="K96" s="22"/>
+      <c r="L96" s="22"/>
+      <c r="M96" s="22"/>
     </row>
     <row r="97">
       <c r="A97" s="19" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C97" s="19" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="D97" s="8" t="s">
         <v>111</v>
@@ -7357,61 +7867,81 @@
       <c r="F97" s="22"/>
       <c r="G97" s="22"/>
       <c r="H97" s="22"/>
+      <c r="I97" s="22"/>
+      <c r="J97" s="22"/>
+      <c r="K97" s="22"/>
+      <c r="L97" s="22"/>
+      <c r="M97" s="22"/>
     </row>
     <row r="98">
       <c r="C98" s="19" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="D98" s="8" t="s">
         <v>114</v>
       </c>
       <c r="E98" s="8" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F98" s="22"/>
       <c r="G98" s="22"/>
       <c r="H98" s="22"/>
+      <c r="I98" s="22"/>
+      <c r="J98" s="22"/>
+      <c r="K98" s="22"/>
+      <c r="L98" s="22"/>
+      <c r="M98" s="22"/>
     </row>
     <row r="99">
       <c r="B99" s="7" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C99" s="19" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="D99" s="8" t="s">
         <v>145</v>
       </c>
       <c r="E99" s="8" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="F99" s="22"/>
       <c r="G99" s="22"/>
       <c r="H99" s="22"/>
+      <c r="I99" s="22"/>
+      <c r="J99" s="22"/>
+      <c r="K99" s="22"/>
+      <c r="L99" s="22"/>
+      <c r="M99" s="22"/>
     </row>
     <row r="100">
       <c r="B100" s="7" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C100" s="19" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="D100" s="8" t="s">
         <v>147</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="F100" s="22"/>
       <c r="G100" s="22"/>
       <c r="H100" s="22"/>
+      <c r="I100" s="22"/>
+      <c r="J100" s="22"/>
+      <c r="K100" s="22"/>
+      <c r="L100" s="22"/>
+      <c r="M100" s="22"/>
     </row>
     <row r="101">
       <c r="B101" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C101" s="19" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="D101" s="8" t="s">
         <v>102</v>
@@ -7422,181 +7952,246 @@
       <c r="F101" s="22"/>
       <c r="G101" s="22"/>
       <c r="H101" s="22"/>
+      <c r="I101" s="22"/>
+      <c r="J101" s="22"/>
+      <c r="K101" s="22"/>
+      <c r="L101" s="22"/>
+      <c r="M101" s="22"/>
     </row>
     <row r="102">
       <c r="C102" s="19" t="s">
-        <v>541</v>
-      </c>
-      <c r="D102" s="8" t="s">
-        <v>542</v>
-      </c>
-      <c r="E102" s="8" t="s">
-        <v>193</v>
+        <v>539</v>
+      </c>
+      <c r="D102" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E102" s="24" t="s">
+        <v>540</v>
       </c>
       <c r="F102" s="22"/>
       <c r="G102" s="22"/>
       <c r="H102" s="22"/>
+      <c r="I102" s="22"/>
+      <c r="J102" s="22"/>
+      <c r="K102" s="22"/>
+      <c r="L102" s="22"/>
+      <c r="M102" s="22"/>
     </row>
     <row r="103">
       <c r="C103" s="19" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D103" s="24" t="s">
-        <v>544</v>
-      </c>
-      <c r="E103" s="8" t="s">
-        <v>195</v>
+        <v>520</v>
+      </c>
+      <c r="E103" s="24" t="s">
+        <v>542</v>
       </c>
       <c r="F103" s="22"/>
       <c r="G103" s="22"/>
       <c r="H103" s="22"/>
+      <c r="I103" s="22"/>
+      <c r="J103" s="22"/>
+      <c r="K103" s="22"/>
+      <c r="L103" s="22"/>
+      <c r="M103" s="22"/>
     </row>
     <row r="104">
       <c r="C104" s="19" t="s">
-        <v>545</v>
-      </c>
-      <c r="D104" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="E104" s="8" t="s">
-        <v>546</v>
+        <v>543</v>
+      </c>
+      <c r="D104" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="E104" s="24" t="s">
+        <v>544</v>
       </c>
       <c r="F104" s="22"/>
       <c r="G104" s="22"/>
       <c r="H104" s="22"/>
+      <c r="I104" s="22"/>
+      <c r="J104" s="22"/>
+      <c r="K104" s="22"/>
+      <c r="L104" s="22"/>
+      <c r="M104" s="22"/>
     </row>
     <row r="105">
       <c r="C105" s="19" t="s">
+        <v>545</v>
+      </c>
+      <c r="D105" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="E105" s="5" t="s">
         <v>547</v>
       </c>
-      <c r="D105" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>280</v>
-      </c>
       <c r="F105" s="22"/>
-      <c r="G105" s="22"/>
-      <c r="H105" s="22"/>
+      <c r="G105" s="25"/>
+      <c r="H105" s="24"/>
+      <c r="I105" s="24"/>
+      <c r="J105" s="26"/>
+      <c r="K105" s="26"/>
+      <c r="L105" s="26"/>
+      <c r="M105" s="22"/>
     </row>
     <row r="106">
       <c r="C106" s="19" t="s">
         <v>548</v>
       </c>
-      <c r="D106" s="8" t="s">
-        <v>549</v>
-      </c>
-      <c r="E106" s="8" t="s">
-        <v>203</v>
+      <c r="D106" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E106" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="F106" s="22"/>
-      <c r="G106" s="22"/>
-      <c r="H106" s="22"/>
+      <c r="G106" s="27"/>
+      <c r="H106" s="25"/>
+      <c r="I106" s="24"/>
+      <c r="J106" s="24"/>
+      <c r="K106" s="26"/>
+      <c r="L106" s="26"/>
+      <c r="M106" s="26"/>
     </row>
     <row r="107">
       <c r="C107" s="19" t="s">
+        <v>549</v>
+      </c>
+      <c r="D107" s="5" t="s">
         <v>550</v>
       </c>
-      <c r="D107" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="E107" s="8" t="s">
-        <v>197</v>
+      <c r="E107" s="5" t="s">
+        <v>551</v>
       </c>
       <c r="F107" s="22"/>
-      <c r="G107" s="22"/>
-      <c r="H107" s="22"/>
+      <c r="G107" s="27"/>
+      <c r="H107" s="25"/>
+      <c r="I107" s="24"/>
+      <c r="J107" s="24"/>
+      <c r="K107" s="26"/>
+      <c r="L107" s="26"/>
+      <c r="M107" s="26"/>
     </row>
     <row r="108">
       <c r="C108" s="19" t="s">
-        <v>551</v>
-      </c>
-      <c r="D108" s="8" t="s">
-        <v>198</v>
-      </c>
-      <c r="E108" s="8" t="s">
-        <v>195</v>
+        <v>552</v>
+      </c>
+      <c r="D108" s="28" t="s">
+        <v>553</v>
+      </c>
+      <c r="E108" s="5" t="s">
+        <v>554</v>
       </c>
       <c r="F108" s="22"/>
-      <c r="G108" s="22"/>
-      <c r="H108" s="22"/>
+      <c r="G108" s="27"/>
+      <c r="H108" s="25"/>
+      <c r="I108" s="24"/>
+      <c r="J108" s="24"/>
+      <c r="K108" s="26"/>
+      <c r="L108" s="26"/>
+      <c r="M108" s="26"/>
     </row>
     <row r="109">
       <c r="C109" s="19" t="s">
-        <v>552</v>
-      </c>
-      <c r="D109" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="E109" s="8" t="s">
-        <v>167</v>
+        <v>555</v>
+      </c>
+      <c r="D109" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="E109" s="5" t="s">
+        <v>287</v>
       </c>
       <c r="F109" s="22"/>
-      <c r="G109" s="22"/>
-      <c r="H109" s="22"/>
+      <c r="G109" s="27"/>
+      <c r="H109" s="25"/>
+      <c r="I109" s="24"/>
+      <c r="J109" s="24"/>
+      <c r="K109" s="26"/>
+      <c r="L109" s="26"/>
+      <c r="M109" s="26"/>
     </row>
     <row r="110">
       <c r="C110" s="19" t="s">
-        <v>553</v>
-      </c>
-      <c r="D110" s="8" t="s">
-        <v>168</v>
-      </c>
-      <c r="E110" s="8" t="s">
-        <v>169</v>
+        <v>556</v>
+      </c>
+      <c r="D110" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="E110" s="19" t="s">
+        <v>280</v>
       </c>
       <c r="F110" s="22"/>
-      <c r="G110" s="22"/>
-      <c r="H110" s="22"/>
+      <c r="G110" s="27"/>
+      <c r="H110" s="25"/>
+      <c r="I110" s="24"/>
+      <c r="J110" s="24"/>
+      <c r="K110" s="26"/>
+      <c r="L110" s="26"/>
+      <c r="M110" s="26"/>
     </row>
     <row r="111">
       <c r="C111" s="19" t="s">
-        <v>554</v>
-      </c>
-      <c r="D111" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="E111" s="8" t="s">
-        <v>135</v>
+        <v>557</v>
+      </c>
+      <c r="D111" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="E111" s="19" t="s">
+        <v>559</v>
       </c>
       <c r="F111" s="22"/>
-      <c r="G111" s="22"/>
-      <c r="H111" s="22"/>
+      <c r="G111" s="27"/>
+      <c r="H111" s="25"/>
+      <c r="I111" s="24"/>
+      <c r="J111" s="24"/>
+      <c r="K111" s="26"/>
+      <c r="L111" s="26"/>
+      <c r="M111" s="26"/>
     </row>
     <row r="112">
       <c r="C112" s="19" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="D112" s="8" t="s">
-        <v>109</v>
+        <v>196</v>
       </c>
       <c r="E112" s="8" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
       <c r="F112" s="22"/>
-      <c r="G112" s="22"/>
-      <c r="H112" s="22"/>
+      <c r="G112" s="27"/>
+      <c r="H112" s="25"/>
+      <c r="I112" s="24"/>
+      <c r="J112" s="24"/>
+      <c r="K112" s="26"/>
+      <c r="L112" s="26"/>
+      <c r="M112" s="26"/>
     </row>
     <row r="113">
       <c r="C113" s="19" t="s">
-        <v>556</v>
-      </c>
-      <c r="D113" s="3" t="s">
+        <v>561</v>
+      </c>
+      <c r="D113" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="E113" s="3" t="s">
-        <v>557</v>
+      <c r="E113" s="8" t="s">
+        <v>195</v>
       </c>
       <c r="F113" s="22"/>
-      <c r="G113" s="22"/>
-      <c r="H113" s="22"/>
+      <c r="G113" s="27"/>
+      <c r="H113" s="25"/>
+      <c r="I113" s="24"/>
+      <c r="J113" s="24"/>
+      <c r="K113" s="26"/>
+      <c r="L113" s="26"/>
+      <c r="M113" s="26"/>
     </row>
     <row r="114">
       <c r="B114" s="19" t="s">
         <v>395</v>
       </c>
       <c r="C114" s="19" t="s">
-        <v>558</v>
+        <v>562</v>
       </c>
       <c r="D114" s="3" t="s">
         <v>166</v>
@@ -7605,12 +8200,17 @@
         <v>167</v>
       </c>
       <c r="F114" s="22"/>
-      <c r="G114" s="22"/>
-      <c r="H114" s="22"/>
+      <c r="G114" s="27"/>
+      <c r="H114" s="25"/>
+      <c r="I114" s="24"/>
+      <c r="J114" s="24"/>
+      <c r="K114" s="26"/>
+      <c r="L114" s="26"/>
+      <c r="M114" s="26"/>
     </row>
     <row r="115">
       <c r="C115" s="19" t="s">
-        <v>559</v>
+        <v>563</v>
       </c>
       <c r="D115" s="3" t="s">
         <v>168</v>
@@ -7619,18 +8219,23 @@
         <v>169</v>
       </c>
       <c r="F115" s="22"/>
-      <c r="G115" s="22"/>
-      <c r="H115" s="22"/>
+      <c r="G115" s="27"/>
+      <c r="H115" s="25"/>
+      <c r="I115" s="24"/>
+      <c r="J115" s="24"/>
+      <c r="K115" s="26"/>
+      <c r="L115" s="26"/>
+      <c r="M115" s="26"/>
     </row>
     <row r="116">
       <c r="A116" s="16" t="s">
-        <v>560</v>
+        <v>564</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C116" s="16" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="D116" s="3" t="s">
         <v>134</v>
@@ -7639,12 +8244,17 @@
         <v>313</v>
       </c>
       <c r="F116" s="22"/>
-      <c r="G116" s="22"/>
-      <c r="H116" s="22"/>
+      <c r="G116" s="27"/>
+      <c r="H116" s="25"/>
+      <c r="I116" s="24"/>
+      <c r="J116" s="24"/>
+      <c r="K116" s="26"/>
+      <c r="L116" s="26"/>
+      <c r="M116" s="26"/>
     </row>
     <row r="117">
       <c r="C117" s="16" t="s">
-        <v>562</v>
+        <v>566</v>
       </c>
       <c r="D117" s="3" t="s">
         <v>109</v>
@@ -7653,26 +8263,36 @@
         <v>110</v>
       </c>
       <c r="F117" s="22"/>
-      <c r="G117" s="22"/>
-      <c r="H117" s="22"/>
+      <c r="G117" s="27"/>
+      <c r="H117" s="25"/>
+      <c r="I117" s="24"/>
+      <c r="J117" s="24"/>
+      <c r="K117" s="22"/>
+      <c r="L117" s="22"/>
+      <c r="M117" s="22"/>
     </row>
     <row r="118">
       <c r="C118" s="16" t="s">
-        <v>563</v>
+        <v>567</v>
       </c>
       <c r="D118" s="8" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>565</v>
+        <v>569</v>
       </c>
       <c r="F118" s="22"/>
-      <c r="G118" s="22"/>
+      <c r="G118" s="29"/>
       <c r="H118" s="22"/>
+      <c r="I118" s="22"/>
+      <c r="J118" s="22"/>
+      <c r="K118" s="22"/>
+      <c r="L118" s="22"/>
+      <c r="M118" s="22"/>
     </row>
     <row r="119">
       <c r="C119" s="19" t="s">
-        <v>566</v>
+        <v>570</v>
       </c>
       <c r="D119" s="8" t="s">
         <v>353</v>
@@ -7683,10 +8303,15 @@
       <c r="F119" s="22"/>
       <c r="G119" s="22"/>
       <c r="H119" s="22"/>
+      <c r="I119" s="22"/>
+      <c r="J119" s="22"/>
+      <c r="K119" s="22"/>
+      <c r="L119" s="22"/>
+      <c r="M119" s="22"/>
     </row>
     <row r="120">
       <c r="C120" s="16" t="s">
-        <v>567</v>
+        <v>571</v>
       </c>
       <c r="D120" s="8" t="s">
         <v>136</v>
@@ -7697,10 +8322,15 @@
       <c r="F120" s="22"/>
       <c r="G120" s="22"/>
       <c r="H120" s="22"/>
+      <c r="I120" s="22"/>
+      <c r="J120" s="22"/>
+      <c r="K120" s="22"/>
+      <c r="L120" s="22"/>
+      <c r="M120" s="22"/>
     </row>
     <row r="121">
       <c r="C121" s="16" t="s">
-        <v>568</v>
+        <v>572</v>
       </c>
       <c r="D121" s="8" t="s">
         <v>149</v>
@@ -7711,10 +8341,15 @@
       <c r="F121" s="22"/>
       <c r="G121" s="22"/>
       <c r="H121" s="22"/>
+      <c r="I121" s="22"/>
+      <c r="J121" s="22"/>
+      <c r="K121" s="22"/>
+      <c r="L121" s="22"/>
+      <c r="M121" s="22"/>
     </row>
     <row r="122">
       <c r="C122" s="16" t="s">
-        <v>569</v>
+        <v>573</v>
       </c>
       <c r="D122" s="8" t="s">
         <v>151</v>
@@ -7725,10 +8360,15 @@
       <c r="F122" s="22"/>
       <c r="G122" s="22"/>
       <c r="H122" s="22"/>
+      <c r="I122" s="22"/>
+      <c r="J122" s="22"/>
+      <c r="K122" s="22"/>
+      <c r="L122" s="22"/>
+      <c r="M122" s="22"/>
     </row>
     <row r="123">
       <c r="C123" s="16" t="s">
-        <v>570</v>
+        <v>574</v>
       </c>
       <c r="D123" s="8" t="s">
         <v>153</v>
@@ -7739,10 +8379,15 @@
       <c r="F123" s="22"/>
       <c r="G123" s="22"/>
       <c r="H123" s="22"/>
+      <c r="I123" s="22"/>
+      <c r="J123" s="22"/>
+      <c r="K123" s="22"/>
+      <c r="L123" s="22"/>
+      <c r="M123" s="22"/>
     </row>
     <row r="124">
       <c r="C124" s="16" t="s">
-        <v>571</v>
+        <v>575</v>
       </c>
       <c r="D124" s="8" t="s">
         <v>116</v>
@@ -7753,27 +8398,37 @@
       <c r="F124" s="22"/>
       <c r="G124" s="22"/>
       <c r="H124" s="22"/>
+      <c r="I124" s="22"/>
+      <c r="J124" s="22"/>
+      <c r="K124" s="22"/>
+      <c r="L124" s="22"/>
+      <c r="M124" s="22"/>
     </row>
     <row r="125">
       <c r="B125" s="16" t="s">
         <v>395</v>
       </c>
       <c r="C125" s="16" t="s">
-        <v>572</v>
+        <v>576</v>
       </c>
       <c r="D125" s="8" t="s">
         <v>316</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>573</v>
+        <v>577</v>
       </c>
       <c r="F125" s="22"/>
       <c r="G125" s="22"/>
       <c r="H125" s="22"/>
+      <c r="I125" s="22"/>
+      <c r="J125" s="22"/>
+      <c r="K125" s="22"/>
+      <c r="L125" s="22"/>
+      <c r="M125" s="22"/>
     </row>
     <row r="126">
       <c r="C126" s="16" t="s">
-        <v>574</v>
+        <v>578</v>
       </c>
       <c r="D126" s="8" t="s">
         <v>322</v>
@@ -7784,69 +8439,94 @@
       <c r="F126" s="22"/>
       <c r="G126" s="22"/>
       <c r="H126" s="22"/>
+      <c r="I126" s="22"/>
+      <c r="J126" s="22"/>
+      <c r="K126" s="22"/>
+      <c r="L126" s="22"/>
+      <c r="M126" s="22"/>
     </row>
     <row r="127">
-      <c r="C127" s="25" t="s">
-        <v>575</v>
+      <c r="C127" s="30" t="s">
+        <v>579</v>
       </c>
       <c r="D127" s="8" t="s">
         <v>350</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>576</v>
+        <v>580</v>
       </c>
       <c r="F127" s="22"/>
       <c r="G127" s="22"/>
       <c r="H127" s="22"/>
+      <c r="I127" s="22"/>
+      <c r="J127" s="22"/>
+      <c r="K127" s="22"/>
+      <c r="L127" s="22"/>
+      <c r="M127" s="22"/>
     </row>
     <row r="128">
       <c r="C128" s="16" t="s">
-        <v>577</v>
+        <v>581</v>
       </c>
       <c r="D128" s="8" t="s">
         <v>346</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>578</v>
+        <v>582</v>
       </c>
       <c r="F128" s="22"/>
       <c r="G128" s="22"/>
       <c r="H128" s="22"/>
+      <c r="I128" s="22"/>
+      <c r="J128" s="22"/>
+      <c r="K128" s="22"/>
+      <c r="L128" s="22"/>
+      <c r="M128" s="22"/>
     </row>
     <row r="129">
       <c r="B129" s="16" t="s">
         <v>453</v>
       </c>
       <c r="C129" s="16" t="s">
-        <v>579</v>
+        <v>583</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="F129" s="22"/>
       <c r="G129" s="22"/>
       <c r="H129" s="22"/>
+      <c r="I129" s="22"/>
+      <c r="J129" s="22"/>
+      <c r="K129" s="22"/>
+      <c r="L129" s="22"/>
+      <c r="M129" s="22"/>
     </row>
     <row r="130">
       <c r="C130" s="16" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>371</v>
-      </c>
-      <c r="E130" s="8" t="s">
-        <v>583</v>
+        <v>587</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>588</v>
       </c>
       <c r="F130" s="22"/>
       <c r="G130" s="22"/>
       <c r="H130" s="22"/>
+      <c r="I130" s="22"/>
+      <c r="J130" s="22"/>
+      <c r="K130" s="22"/>
+      <c r="L130" s="22"/>
+      <c r="M130" s="22"/>
     </row>
     <row r="131">
       <c r="C131" s="16" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="D131" s="7" t="s">
         <v>366</v>
@@ -7857,80 +8537,110 @@
       <c r="F131" s="22"/>
       <c r="G131" s="22"/>
       <c r="H131" s="22"/>
+      <c r="I131" s="22"/>
+      <c r="J131" s="22"/>
+      <c r="K131" s="22"/>
+      <c r="L131" s="22"/>
+      <c r="M131" s="22"/>
     </row>
     <row r="132">
       <c r="C132" s="16" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="D132" s="8" t="s">
         <v>368</v>
       </c>
-      <c r="E132" s="8" t="s">
-        <v>586</v>
+      <c r="E132" s="3" t="s">
+        <v>369</v>
       </c>
       <c r="F132" s="22"/>
       <c r="G132" s="22"/>
       <c r="H132" s="22"/>
+      <c r="I132" s="22"/>
+      <c r="J132" s="22"/>
+      <c r="K132" s="22"/>
+      <c r="L132" s="22"/>
+      <c r="M132" s="22"/>
     </row>
     <row r="133">
       <c r="C133" s="16" t="s">
-        <v>587</v>
+        <v>591</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>588</v>
+        <v>592</v>
       </c>
       <c r="E133" s="8" t="s">
-        <v>589</v>
+        <v>593</v>
       </c>
       <c r="F133" s="22"/>
       <c r="G133" s="22"/>
       <c r="H133" s="22"/>
+      <c r="I133" s="22"/>
+      <c r="J133" s="22"/>
+      <c r="K133" s="22"/>
+      <c r="L133" s="22"/>
+      <c r="M133" s="22"/>
     </row>
     <row r="134">
       <c r="C134" s="16" t="s">
-        <v>590</v>
+        <v>594</v>
       </c>
       <c r="D134" s="8" t="s">
         <v>332</v>
       </c>
       <c r="E134" s="8" t="s">
-        <v>591</v>
+        <v>595</v>
       </c>
       <c r="F134" s="22"/>
       <c r="G134" s="22"/>
       <c r="H134" s="22"/>
+      <c r="I134" s="22"/>
+      <c r="J134" s="22"/>
+      <c r="K134" s="22"/>
+      <c r="L134" s="22"/>
+      <c r="M134" s="22"/>
     </row>
     <row r="135">
       <c r="C135" s="16" t="s">
-        <v>592</v>
+        <v>596</v>
       </c>
       <c r="D135" s="8" t="s">
         <v>335</v>
       </c>
       <c r="E135" s="8" t="s">
-        <v>593</v>
+        <v>597</v>
       </c>
       <c r="F135" s="22"/>
       <c r="G135" s="22"/>
       <c r="H135" s="22"/>
+      <c r="I135" s="22"/>
+      <c r="J135" s="22"/>
+      <c r="K135" s="22"/>
+      <c r="L135" s="22"/>
+      <c r="M135" s="22"/>
     </row>
     <row r="136">
       <c r="C136" s="16" t="s">
-        <v>594</v>
+        <v>598</v>
       </c>
       <c r="D136" s="8" t="s">
         <v>337</v>
       </c>
       <c r="E136" s="8" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
       <c r="F136" s="22"/>
       <c r="G136" s="22"/>
       <c r="H136" s="22"/>
+      <c r="I136" s="22"/>
+      <c r="J136" s="22"/>
+      <c r="K136" s="22"/>
+      <c r="L136" s="22"/>
+      <c r="M136" s="22"/>
     </row>
     <row r="137">
       <c r="C137" s="16" t="s">
-        <v>596</v>
+        <v>600</v>
       </c>
       <c r="D137" s="8" t="s">
         <v>340</v>
@@ -7941,38 +8651,53 @@
       <c r="F137" s="22"/>
       <c r="G137" s="22"/>
       <c r="H137" s="22"/>
+      <c r="I137" s="22"/>
+      <c r="J137" s="22"/>
+      <c r="K137" s="22"/>
+      <c r="L137" s="22"/>
+      <c r="M137" s="22"/>
     </row>
     <row r="138">
       <c r="C138" s="16" t="s">
-        <v>597</v>
+        <v>601</v>
       </c>
       <c r="D138" s="8" t="s">
         <v>343</v>
       </c>
       <c r="E138" s="8" t="s">
-        <v>598</v>
+        <v>602</v>
       </c>
       <c r="F138" s="22"/>
       <c r="G138" s="22"/>
       <c r="H138" s="22"/>
+      <c r="I138" s="22"/>
+      <c r="J138" s="22"/>
+      <c r="K138" s="22"/>
+      <c r="L138" s="22"/>
+      <c r="M138" s="22"/>
     </row>
     <row r="139">
       <c r="C139" s="16" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="D139" s="8" t="s">
         <v>348</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>600</v>
+        <v>604</v>
       </c>
       <c r="F139" s="22"/>
       <c r="G139" s="22"/>
       <c r="H139" s="22"/>
+      <c r="I139" s="22"/>
+      <c r="J139" s="22"/>
+      <c r="K139" s="22"/>
+      <c r="L139" s="22"/>
+      <c r="M139" s="22"/>
     </row>
     <row r="140">
       <c r="C140" s="16" t="s">
-        <v>601</v>
+        <v>605</v>
       </c>
       <c r="D140" s="8" t="s">
         <v>355</v>
@@ -7983,10 +8708,15 @@
       <c r="F140" s="22"/>
       <c r="G140" s="22"/>
       <c r="H140" s="22"/>
+      <c r="I140" s="22"/>
+      <c r="J140" s="22"/>
+      <c r="K140" s="22"/>
+      <c r="L140" s="22"/>
+      <c r="M140" s="22"/>
     </row>
     <row r="141">
       <c r="C141" s="19" t="s">
-        <v>602</v>
+        <v>606</v>
       </c>
       <c r="D141" s="8" t="s">
         <v>361</v>
@@ -7997,10 +8727,15 @@
       <c r="F141" s="22"/>
       <c r="G141" s="22"/>
       <c r="H141" s="22"/>
+      <c r="I141" s="22"/>
+      <c r="J141" s="22"/>
+      <c r="K141" s="22"/>
+      <c r="L141" s="22"/>
+      <c r="M141" s="22"/>
     </row>
     <row r="142">
       <c r="C142" s="19" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="D142" s="8" t="s">
         <v>260</v>
@@ -8011,16 +8746,21 @@
       <c r="F142" s="22"/>
       <c r="G142" s="22"/>
       <c r="H142" s="22"/>
+      <c r="I142" s="22"/>
+      <c r="J142" s="22"/>
+      <c r="K142" s="22"/>
+      <c r="L142" s="22"/>
+      <c r="M142" s="22"/>
     </row>
     <row r="143">
       <c r="A143" s="19" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="B143" s="19" t="s">
         <v>395</v>
       </c>
       <c r="C143" s="19" t="s">
-        <v>605</v>
+        <v>609</v>
       </c>
       <c r="D143" s="8" t="s">
         <v>272</v>
@@ -8031,13 +8771,18 @@
       <c r="F143" s="22"/>
       <c r="G143" s="22"/>
       <c r="H143" s="22"/>
+      <c r="I143" s="22"/>
+      <c r="J143" s="22"/>
+      <c r="K143" s="22"/>
+      <c r="L143" s="22"/>
+      <c r="M143" s="22"/>
     </row>
     <row r="144">
       <c r="B144" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C144" s="19" t="s">
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="D144" s="8" t="s">
         <v>270</v>
@@ -8048,30 +8793,40 @@
       <c r="F144" s="22"/>
       <c r="G144" s="22"/>
       <c r="H144" s="22"/>
+      <c r="I144" s="22"/>
+      <c r="J144" s="22"/>
+      <c r="K144" s="22"/>
+      <c r="L144" s="22"/>
+      <c r="M144" s="22"/>
     </row>
     <row r="145">
       <c r="C145" s="19" t="s">
-        <v>607</v>
+        <v>611</v>
       </c>
       <c r="D145" s="8" t="s">
         <v>274</v>
       </c>
       <c r="E145" s="8" t="s">
-        <v>608</v>
+        <v>612</v>
       </c>
       <c r="F145" s="22"/>
       <c r="G145" s="22"/>
       <c r="H145" s="22"/>
+      <c r="I145" s="22"/>
+      <c r="J145" s="22"/>
+      <c r="K145" s="22"/>
+      <c r="L145" s="22"/>
+      <c r="M145" s="22"/>
     </row>
     <row r="146">
       <c r="A146" s="19" t="s">
-        <v>609</v>
+        <v>613</v>
       </c>
       <c r="B146" s="19" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C146" s="19" t="s">
-        <v>610</v>
+        <v>614</v>
       </c>
       <c r="D146" s="8" t="s">
         <v>80</v>
@@ -8082,10 +8837,15 @@
       <c r="F146" s="22"/>
       <c r="G146" s="22"/>
       <c r="H146" s="22"/>
+      <c r="I146" s="22"/>
+      <c r="J146" s="22"/>
+      <c r="K146" s="22"/>
+      <c r="L146" s="22"/>
+      <c r="M146" s="22"/>
     </row>
     <row r="147">
       <c r="C147" s="19" t="s">
-        <v>611</v>
+        <v>615</v>
       </c>
       <c r="D147" s="8" t="s">
         <v>91</v>
@@ -8096,41 +8856,56 @@
       <c r="F147" s="22"/>
       <c r="G147" s="22"/>
       <c r="H147" s="22"/>
+      <c r="I147" s="22"/>
+      <c r="J147" s="22"/>
+      <c r="K147" s="22"/>
+      <c r="L147" s="22"/>
+      <c r="M147" s="22"/>
     </row>
     <row r="148">
       <c r="C148" s="19" t="s">
-        <v>612</v>
+        <v>616</v>
       </c>
       <c r="D148" s="3" t="s">
         <v>88</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
       <c r="F148" s="22"/>
       <c r="G148" s="22"/>
       <c r="H148" s="22"/>
+      <c r="I148" s="22"/>
+      <c r="J148" s="22"/>
+      <c r="K148" s="22"/>
+      <c r="L148" s="22"/>
+      <c r="M148" s="22"/>
     </row>
     <row r="149">
       <c r="C149" s="7" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="F149" s="22"/>
       <c r="G149" s="22"/>
       <c r="H149" s="22"/>
+      <c r="I149" s="22"/>
+      <c r="J149" s="22"/>
+      <c r="K149" s="22"/>
+      <c r="L149" s="22"/>
+      <c r="M149" s="22"/>
     </row>
     <row r="150">
       <c r="B150" s="19" t="s">
         <v>395</v>
       </c>
       <c r="C150" s="7" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="D150" s="3" t="s">
         <v>236</v>
@@ -8141,10 +8916,15 @@
       <c r="F150" s="22"/>
       <c r="G150" s="22"/>
       <c r="H150" s="22"/>
+      <c r="I150" s="22"/>
+      <c r="J150" s="22"/>
+      <c r="K150" s="22"/>
+      <c r="L150" s="22"/>
+      <c r="M150" s="22"/>
     </row>
     <row r="151">
       <c r="C151" s="7" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="D151" s="3" t="s">
         <v>364</v>
@@ -8155,10 +8935,15 @@
       <c r="F151" s="22"/>
       <c r="G151" s="22"/>
       <c r="H151" s="22"/>
+      <c r="I151" s="22"/>
+      <c r="J151" s="22"/>
+      <c r="K151" s="22"/>
+      <c r="L151" s="22"/>
+      <c r="M151" s="22"/>
     </row>
     <row r="152">
       <c r="C152" s="7" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="D152" s="3" t="s">
         <v>209</v>
@@ -8169,10 +8954,15 @@
       <c r="F152" s="22"/>
       <c r="G152" s="22"/>
       <c r="H152" s="22"/>
+      <c r="I152" s="22"/>
+      <c r="J152" s="22"/>
+      <c r="K152" s="22"/>
+      <c r="L152" s="22"/>
+      <c r="M152" s="22"/>
     </row>
     <row r="153">
       <c r="C153" s="7" t="s">
-        <v>620</v>
+        <v>624</v>
       </c>
       <c r="D153" s="3" t="s">
         <v>84</v>
@@ -8183,10 +8973,15 @@
       <c r="F153" s="22"/>
       <c r="G153" s="22"/>
       <c r="H153" s="22"/>
+      <c r="I153" s="22"/>
+      <c r="J153" s="22"/>
+      <c r="K153" s="22"/>
+      <c r="L153" s="22"/>
+      <c r="M153" s="22"/>
     </row>
     <row r="154">
       <c r="C154" s="7" t="s">
-        <v>621</v>
+        <v>625</v>
       </c>
       <c r="D154" s="3" t="s">
         <v>215</v>
@@ -8197,10 +8992,15 @@
       <c r="F154" s="22"/>
       <c r="G154" s="22"/>
       <c r="H154" s="22"/>
+      <c r="I154" s="22"/>
+      <c r="J154" s="22"/>
+      <c r="K154" s="22"/>
+      <c r="L154" s="22"/>
+      <c r="M154" s="22"/>
     </row>
     <row r="155">
       <c r="C155" s="7" t="s">
-        <v>622</v>
+        <v>626</v>
       </c>
       <c r="D155" s="3" t="s">
         <v>217</v>
@@ -8211,69 +9011,94 @@
       <c r="F155" s="22"/>
       <c r="G155" s="22"/>
       <c r="H155" s="22"/>
+      <c r="I155" s="22"/>
+      <c r="J155" s="22"/>
+      <c r="K155" s="22"/>
+      <c r="L155" s="22"/>
+      <c r="M155" s="22"/>
     </row>
     <row r="156">
       <c r="B156" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C156" s="19" t="s">
-        <v>623</v>
+        <v>627</v>
       </c>
       <c r="D156" s="3" t="s">
         <v>220</v>
       </c>
-      <c r="E156" s="3" t="s">
-        <v>221</v>
+      <c r="E156" s="7" t="s">
+        <v>255</v>
       </c>
       <c r="F156" s="22"/>
       <c r="G156" s="22"/>
       <c r="H156" s="22"/>
+      <c r="I156" s="22"/>
+      <c r="J156" s="22"/>
+      <c r="K156" s="22"/>
+      <c r="L156" s="22"/>
+      <c r="M156" s="22"/>
     </row>
     <row r="157">
       <c r="C157" s="19" t="s">
-        <v>624</v>
+        <v>628</v>
       </c>
       <c r="D157" s="3" t="s">
         <v>252</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>625</v>
+        <v>629</v>
       </c>
       <c r="F157" s="22"/>
       <c r="G157" s="22"/>
       <c r="H157" s="22"/>
+      <c r="I157" s="22"/>
+      <c r="J157" s="22"/>
+      <c r="K157" s="22"/>
+      <c r="L157" s="22"/>
+      <c r="M157" s="22"/>
     </row>
     <row r="158">
       <c r="C158" s="19" t="s">
-        <v>626</v>
+        <v>630</v>
       </c>
       <c r="D158" s="10" t="s">
-        <v>627</v>
+        <v>631</v>
       </c>
       <c r="E158" s="10" t="s">
-        <v>628</v>
+        <v>632</v>
       </c>
       <c r="F158" s="22"/>
       <c r="G158" s="22"/>
       <c r="H158" s="22"/>
+      <c r="I158" s="22"/>
+      <c r="J158" s="22"/>
+      <c r="K158" s="22"/>
+      <c r="L158" s="22"/>
+      <c r="M158" s="22"/>
     </row>
     <row r="159">
       <c r="C159" s="19" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
       <c r="D159" s="3" t="s">
         <v>207</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>630</v>
+        <v>634</v>
       </c>
       <c r="F159" s="22"/>
       <c r="G159" s="22"/>
       <c r="H159" s="22"/>
+      <c r="I159" s="22"/>
+      <c r="J159" s="22"/>
+      <c r="K159" s="22"/>
+      <c r="L159" s="22"/>
+      <c r="M159" s="22"/>
     </row>
     <row r="160">
       <c r="C160" s="19" t="s">
-        <v>631</v>
+        <v>635</v>
       </c>
       <c r="D160" s="3" t="s">
         <v>235</v>
@@ -8284,168 +9109,223 @@
       <c r="F160" s="22"/>
       <c r="G160" s="22"/>
       <c r="H160" s="22"/>
+      <c r="I160" s="22"/>
+      <c r="J160" s="22"/>
+      <c r="K160" s="22"/>
+      <c r="L160" s="22"/>
+      <c r="M160" s="22"/>
     </row>
     <row r="161">
       <c r="C161" s="19" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="F161" s="22"/>
       <c r="G161" s="22"/>
       <c r="H161" s="22"/>
+      <c r="I161" s="22"/>
+      <c r="J161" s="22"/>
+      <c r="K161" s="22"/>
+      <c r="L161" s="22"/>
+      <c r="M161" s="22"/>
     </row>
     <row r="162">
       <c r="B162" s="19" t="s">
         <v>436</v>
       </c>
       <c r="C162" s="7" t="s">
-        <v>635</v>
+        <v>639</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>637</v>
+        <v>641</v>
       </c>
       <c r="F162" s="22"/>
       <c r="G162" s="22"/>
       <c r="H162" s="22"/>
+      <c r="I162" s="22"/>
+      <c r="J162" s="22"/>
+      <c r="K162" s="22"/>
+      <c r="L162" s="22"/>
+      <c r="M162" s="22"/>
     </row>
     <row r="163">
       <c r="C163" s="7" t="s">
-        <v>638</v>
+        <v>642</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>639</v>
+        <v>643</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>640</v>
+        <v>644</v>
       </c>
       <c r="F163" s="22"/>
       <c r="G163" s="22"/>
       <c r="H163" s="22"/>
+      <c r="I163" s="22"/>
+      <c r="J163" s="22"/>
+      <c r="K163" s="22"/>
+      <c r="L163" s="22"/>
+      <c r="M163" s="22"/>
     </row>
     <row r="164">
       <c r="C164" s="7" t="s">
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="D164" s="3" t="s">
         <v>238</v>
       </c>
-      <c r="E164" s="3" t="s">
-        <v>642</v>
+      <c r="E164" s="7" t="s">
+        <v>239</v>
       </c>
       <c r="F164" s="22"/>
       <c r="G164" s="22"/>
       <c r="H164" s="22"/>
+      <c r="I164" s="22"/>
+      <c r="J164" s="22"/>
+      <c r="K164" s="22"/>
+      <c r="L164" s="22"/>
+      <c r="M164" s="22"/>
     </row>
     <row r="165">
       <c r="A165" s="19" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="B165" s="19" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="C165" s="19" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="F165" s="22"/>
       <c r="G165" s="22"/>
       <c r="H165" s="22"/>
+      <c r="I165" s="22"/>
+      <c r="J165" s="22"/>
+      <c r="K165" s="22"/>
+      <c r="L165" s="22"/>
+      <c r="M165" s="22"/>
     </row>
     <row r="166">
       <c r="C166" s="19" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="E166" s="8" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="F166" s="22"/>
       <c r="G166" s="22"/>
       <c r="H166" s="22"/>
+      <c r="I166" s="22"/>
+      <c r="J166" s="22"/>
+      <c r="K166" s="22"/>
+      <c r="L166" s="22"/>
+      <c r="M166" s="22"/>
     </row>
     <row r="167">
       <c r="C167" s="19" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="F167" s="22"/>
       <c r="G167" s="22"/>
       <c r="H167" s="22"/>
+      <c r="I167" s="22"/>
+      <c r="J167" s="22"/>
+      <c r="K167" s="22"/>
+      <c r="L167" s="22"/>
+      <c r="M167" s="22"/>
     </row>
     <row r="168">
       <c r="C168" s="19" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="F168" s="22"/>
       <c r="G168" s="22"/>
       <c r="H168" s="22"/>
+      <c r="I168" s="22"/>
+      <c r="J168" s="22"/>
+      <c r="K168" s="22"/>
+      <c r="L168" s="22"/>
+      <c r="M168" s="22"/>
     </row>
     <row r="169">
       <c r="B169" s="19" t="s">
         <v>436</v>
       </c>
       <c r="C169" s="19" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="E169" s="8" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="F169" s="22"/>
       <c r="G169" s="22"/>
       <c r="H169" s="22"/>
+      <c r="I169" s="22"/>
+      <c r="J169" s="22"/>
+      <c r="K169" s="22"/>
+      <c r="L169" s="22"/>
+      <c r="M169" s="22"/>
     </row>
     <row r="170">
       <c r="C170" s="19" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="F170" s="22"/>
       <c r="G170" s="22"/>
       <c r="H170" s="22"/>
+      <c r="I170" s="22"/>
+      <c r="J170" s="22"/>
+      <c r="K170" s="22"/>
+      <c r="L170" s="22"/>
+      <c r="M170" s="22"/>
     </row>
     <row r="171">
       <c r="A171" s="19" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="B171" s="19" t="s">
         <v>453</v>
       </c>
       <c r="C171" s="19" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="D171" s="3" t="s">
         <v>373</v>
@@ -8456,6 +9336,11 @@
       <c r="F171" s="22"/>
       <c r="G171" s="22"/>
       <c r="H171" s="22"/>
+      <c r="I171" s="22"/>
+      <c r="J171" s="22"/>
+      <c r="K171" s="22"/>
+      <c r="L171" s="22"/>
+      <c r="M171" s="22"/>
     </row>
     <row r="172">
       <c r="A172" s="19"/>
@@ -8465,6 +9350,11 @@
       <c r="F172" s="22"/>
       <c r="G172" s="22"/>
       <c r="H172" s="22"/>
+      <c r="I172" s="22"/>
+      <c r="J172" s="22"/>
+      <c r="K172" s="22"/>
+      <c r="L172" s="22"/>
+      <c r="M172" s="22"/>
     </row>
     <row r="173">
       <c r="A173" s="19"/>
@@ -8475,6 +9365,11 @@
       <c r="F173" s="22"/>
       <c r="G173" s="22"/>
       <c r="H173" s="22"/>
+      <c r="I173" s="22"/>
+      <c r="J173" s="22"/>
+      <c r="K173" s="22"/>
+      <c r="L173" s="22"/>
+      <c r="M173" s="22"/>
     </row>
     <row r="174">
       <c r="A174" s="19"/>
@@ -8484,6 +9379,11 @@
       <c r="F174" s="22"/>
       <c r="G174" s="22"/>
       <c r="H174" s="22"/>
+      <c r="I174" s="22"/>
+      <c r="J174" s="22"/>
+      <c r="K174" s="22"/>
+      <c r="L174" s="22"/>
+      <c r="M174" s="22"/>
     </row>
     <row r="175">
       <c r="A175" s="19"/>
@@ -8492,6 +9392,11 @@
       <c r="F175" s="22"/>
       <c r="G175" s="22"/>
       <c r="H175" s="22"/>
+      <c r="I175" s="22"/>
+      <c r="J175" s="22"/>
+      <c r="K175" s="22"/>
+      <c r="L175" s="22"/>
+      <c r="M175" s="22"/>
     </row>
     <row r="176">
       <c r="A176" s="19"/>
@@ -8501,6 +9406,11 @@
       <c r="F176" s="22"/>
       <c r="G176" s="22"/>
       <c r="H176" s="22"/>
+      <c r="I176" s="22"/>
+      <c r="J176" s="22"/>
+      <c r="K176" s="22"/>
+      <c r="L176" s="22"/>
+      <c r="M176" s="22"/>
     </row>
     <row r="177">
       <c r="A177" s="19"/>
@@ -8509,6 +9419,11 @@
       <c r="F177" s="22"/>
       <c r="G177" s="22"/>
       <c r="H177" s="22"/>
+      <c r="I177" s="22"/>
+      <c r="J177" s="22"/>
+      <c r="K177" s="22"/>
+      <c r="L177" s="22"/>
+      <c r="M177" s="22"/>
     </row>
     <row r="178">
       <c r="A178" s="19"/>
@@ -8517,6 +9432,11 @@
       <c r="F178" s="22"/>
       <c r="G178" s="22"/>
       <c r="H178" s="22"/>
+      <c r="I178" s="22"/>
+      <c r="J178" s="22"/>
+      <c r="K178" s="22"/>
+      <c r="L178" s="22"/>
+      <c r="M178" s="22"/>
     </row>
     <row r="179">
       <c r="A179" s="19"/>
@@ -8525,6 +9445,11 @@
       <c r="F179" s="22"/>
       <c r="G179" s="22"/>
       <c r="H179" s="22"/>
+      <c r="I179" s="22"/>
+      <c r="J179" s="22"/>
+      <c r="K179" s="22"/>
+      <c r="L179" s="22"/>
+      <c r="M179" s="22"/>
     </row>
     <row r="180">
       <c r="A180" s="19"/>
@@ -8533,6 +9458,11 @@
       <c r="F180" s="22"/>
       <c r="G180" s="22"/>
       <c r="H180" s="22"/>
+      <c r="I180" s="22"/>
+      <c r="J180" s="22"/>
+      <c r="K180" s="22"/>
+      <c r="L180" s="22"/>
+      <c r="M180" s="22"/>
     </row>
     <row r="181">
       <c r="A181" s="19"/>
@@ -8541,6 +9471,11 @@
       <c r="F181" s="22"/>
       <c r="G181" s="22"/>
       <c r="H181" s="22"/>
+      <c r="I181" s="22"/>
+      <c r="J181" s="22"/>
+      <c r="K181" s="22"/>
+      <c r="L181" s="22"/>
+      <c r="M181" s="22"/>
     </row>
     <row r="182">
       <c r="A182" s="19"/>
@@ -8549,6 +9484,11 @@
       <c r="F182" s="22"/>
       <c r="G182" s="22"/>
       <c r="H182" s="22"/>
+      <c r="I182" s="22"/>
+      <c r="J182" s="22"/>
+      <c r="K182" s="22"/>
+      <c r="L182" s="22"/>
+      <c r="M182" s="22"/>
     </row>
     <row r="183">
       <c r="A183" s="19"/>
@@ -8557,6 +9497,11 @@
       <c r="F183" s="22"/>
       <c r="G183" s="22"/>
       <c r="H183" s="22"/>
+      <c r="I183" s="22"/>
+      <c r="J183" s="22"/>
+      <c r="K183" s="22"/>
+      <c r="L183" s="22"/>
+      <c r="M183" s="22"/>
     </row>
     <row r="184">
       <c r="A184" s="19"/>
@@ -8565,6 +9510,11 @@
       <c r="F184" s="22"/>
       <c r="G184" s="22"/>
       <c r="H184" s="22"/>
+      <c r="I184" s="22"/>
+      <c r="J184" s="22"/>
+      <c r="K184" s="22"/>
+      <c r="L184" s="22"/>
+      <c r="M184" s="22"/>
     </row>
     <row r="185">
       <c r="A185" s="19"/>
@@ -8573,6 +9523,11 @@
       <c r="F185" s="22"/>
       <c r="G185" s="22"/>
       <c r="H185" s="22"/>
+      <c r="I185" s="22"/>
+      <c r="J185" s="22"/>
+      <c r="K185" s="22"/>
+      <c r="L185" s="22"/>
+      <c r="M185" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="34">

</xml_diff>

<commit_message>
feat: apply new i18n for copy and copied in share link
</commit_message>
<xml_diff>
--- a/scripts/i18n.xlsx
+++ b/scripts/i18n.xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="673">
   <si>
     <t xml:space="preserve">페이지는 [피그마] PFPlay GUI 설계서 합본의 페이지 이름입니다. </t>
   </si>
@@ -1843,6 +1843,9 @@
     <t>party.para.copy_completed</t>
   </si>
   <si>
+    <t>Copied!</t>
+  </si>
+  <si>
     <t>party.para.close_party</t>
   </si>
   <si>
@@ -1882,10 +1885,19 @@
     <t>party.para.enter_confirm_phrase</t>
   </si>
   <si>
+    <t>party.para.share_x_partyroom</t>
+  </si>
+  <si>
+    <t>I'm listening to the {partyroom_name} room. Come hang out!</t>
+  </si>
+  <si>
     <t>party.btn.share_twitter</t>
   </si>
   <si>
     <t>party.btn.copy_link</t>
+  </si>
+  <si>
+    <t>Copy</t>
   </si>
   <si>
     <t>디제잉 (DJ)</t>
@@ -2205,7 +2217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2251,11 +2263,16 @@
       <name val="&quot;Google Sans&quot;"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="NotoSansKR"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2280,6 +2297,12 @@
         <bgColor rgb="FF282C34"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F8F8"/>
+        <bgColor rgb="FFF8F8F8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -2287,7 +2310,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2378,7 +2401,10 @@
     <xf quotePrefix="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -8059,7 +8085,7 @@
         <v>171</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>172</v>
+        <v>550</v>
       </c>
       <c r="F106" s="23"/>
       <c r="G106" s="28"/>
@@ -8072,13 +8098,13 @@
     </row>
     <row r="107">
       <c r="C107" s="20" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F107" s="23"/>
       <c r="G107" s="28"/>
@@ -8091,13 +8117,13 @@
     </row>
     <row r="108">
       <c r="C108" s="20" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D108" s="29" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="F108" s="23"/>
       <c r="G108" s="28"/>
@@ -8110,7 +8136,7 @@
     </row>
     <row r="109">
       <c r="C109" s="20" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>287</v>
@@ -8129,7 +8155,7 @@
     </row>
     <row r="110">
       <c r="C110" s="20" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D110" s="20" t="s">
         <v>281</v>
@@ -8148,13 +8174,13 @@
     </row>
     <row r="111">
       <c r="C111" s="20" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D111" s="20" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E111" s="20" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="F111" s="23"/>
       <c r="G111" s="28"/>
@@ -8167,7 +8193,7 @@
     </row>
     <row r="112">
       <c r="C112" s="20" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>197</v>
@@ -8186,7 +8212,7 @@
     </row>
     <row r="113">
       <c r="C113" s="20" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>199</v>
@@ -8204,17 +8230,15 @@
       <c r="M113" s="27"/>
     </row>
     <row r="114">
-      <c r="B114" s="20" t="s">
-        <v>396</v>
-      </c>
+      <c r="B114" s="20"/>
       <c r="C114" s="20" t="s">
-        <v>563</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>168</v>
+        <v>564</v>
+      </c>
+      <c r="D114" s="30" t="s">
+        <v>565</v>
+      </c>
+      <c r="E114" s="30" t="s">
+        <v>565</v>
       </c>
       <c r="F114" s="23"/>
       <c r="G114" s="28"/>
@@ -8226,14 +8250,17 @@
       <c r="M114" s="27"/>
     </row>
     <row r="115">
+      <c r="B115" s="20" t="s">
+        <v>396</v>
+      </c>
       <c r="C115" s="20" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F115" s="23"/>
       <c r="G115" s="28"/>
@@ -8245,20 +8272,14 @@
       <c r="M115" s="27"/>
     </row>
     <row r="116">
-      <c r="A116" s="17" t="s">
-        <v>565</v>
-      </c>
-      <c r="B116" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="C116" s="17" t="s">
-        <v>566</v>
+      <c r="C116" s="20" t="s">
+        <v>567</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>314</v>
+        <v>568</v>
       </c>
       <c r="F116" s="23"/>
       <c r="G116" s="28"/>
@@ -8270,55 +8291,61 @@
       <c r="M116" s="27"/>
     </row>
     <row r="117">
+      <c r="A117" s="17" t="s">
+        <v>569</v>
+      </c>
+      <c r="B117" s="17" t="s">
+        <v>473</v>
+      </c>
       <c r="C117" s="17" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>111</v>
+        <v>314</v>
       </c>
       <c r="F117" s="23"/>
       <c r="G117" s="28"/>
       <c r="H117" s="26"/>
       <c r="I117" s="25"/>
       <c r="J117" s="25"/>
-      <c r="K117" s="23"/>
-      <c r="L117" s="23"/>
-      <c r="M117" s="23"/>
+      <c r="K117" s="27"/>
+      <c r="L117" s="27"/>
+      <c r="M117" s="27"/>
     </row>
     <row r="118">
       <c r="C118" s="17" t="s">
-        <v>568</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>569</v>
-      </c>
-      <c r="E118" s="8" t="s">
-        <v>570</v>
+        <v>571</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="F118" s="23"/>
-      <c r="G118" s="30"/>
-      <c r="H118" s="23"/>
-      <c r="I118" s="23"/>
-      <c r="J118" s="23"/>
+      <c r="G118" s="28"/>
+      <c r="H118" s="26"/>
+      <c r="I118" s="25"/>
+      <c r="J118" s="25"/>
       <c r="K118" s="23"/>
       <c r="L118" s="23"/>
       <c r="M118" s="23"/>
     </row>
     <row r="119">
-      <c r="C119" s="20" t="s">
-        <v>571</v>
+      <c r="C119" s="17" t="s">
+        <v>572</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>354</v>
+        <v>573</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>355</v>
+        <v>574</v>
       </c>
       <c r="F119" s="23"/>
-      <c r="G119" s="23"/>
+      <c r="G119" s="31"/>
       <c r="H119" s="23"/>
       <c r="I119" s="23"/>
       <c r="J119" s="23"/>
@@ -8327,14 +8354,14 @@
       <c r="M119" s="23"/>
     </row>
     <row r="120">
-      <c r="C120" s="17" t="s">
-        <v>572</v>
+      <c r="C120" s="20" t="s">
+        <v>575</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>137</v>
+        <v>354</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>138</v>
+        <v>355</v>
       </c>
       <c r="F120" s="23"/>
       <c r="G120" s="23"/>
@@ -8347,13 +8374,13 @@
     </row>
     <row r="121">
       <c r="C121" s="17" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F121" s="23"/>
       <c r="G121" s="23"/>
@@ -8366,13 +8393,13 @@
     </row>
     <row r="122">
       <c r="C122" s="17" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F122" s="23"/>
       <c r="G122" s="23"/>
@@ -8385,13 +8412,13 @@
     </row>
     <row r="123">
       <c r="C123" s="17" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F123" s="23"/>
       <c r="G123" s="23"/>
@@ -8404,13 +8431,13 @@
     </row>
     <row r="124">
       <c r="C124" s="17" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="F124" s="23"/>
       <c r="G124" s="23"/>
@@ -8422,17 +8449,14 @@
       <c r="M124" s="23"/>
     </row>
     <row r="125">
-      <c r="B125" s="17" t="s">
-        <v>396</v>
-      </c>
       <c r="C125" s="17" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>317</v>
+        <v>117</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>578</v>
+        <v>118</v>
       </c>
       <c r="F125" s="23"/>
       <c r="G125" s="23"/>
@@ -8444,14 +8468,17 @@
       <c r="M125" s="23"/>
     </row>
     <row r="126">
+      <c r="B126" s="17" t="s">
+        <v>396</v>
+      </c>
       <c r="C126" s="17" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>324</v>
+        <v>582</v>
       </c>
       <c r="F126" s="23"/>
       <c r="G126" s="23"/>
@@ -8463,14 +8490,14 @@
       <c r="M126" s="23"/>
     </row>
     <row r="127">
-      <c r="C127" s="31" t="s">
-        <v>580</v>
+      <c r="C127" s="17" t="s">
+        <v>583</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>581</v>
+        <v>324</v>
       </c>
       <c r="F127" s="23"/>
       <c r="G127" s="23"/>
@@ -8482,14 +8509,14 @@
       <c r="M127" s="23"/>
     </row>
     <row r="128">
-      <c r="C128" s="17" t="s">
-        <v>582</v>
+      <c r="C128" s="32" t="s">
+        <v>584</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="F128" s="23"/>
       <c r="G128" s="23"/>
@@ -8501,17 +8528,14 @@
       <c r="M128" s="23"/>
     </row>
     <row r="129">
-      <c r="B129" s="17" t="s">
-        <v>454</v>
-      </c>
       <c r="C129" s="17" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>585</v>
+        <v>347</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="F129" s="23"/>
       <c r="G129" s="23"/>
@@ -8523,14 +8547,17 @@
       <c r="M129" s="23"/>
     </row>
     <row r="130">
+      <c r="B130" s="17" t="s">
+        <v>454</v>
+      </c>
       <c r="C130" s="17" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>588</v>
-      </c>
-      <c r="E130" s="3" t="s">
         <v>589</v>
+      </c>
+      <c r="E130" s="8" t="s">
+        <v>590</v>
       </c>
       <c r="F130" s="23"/>
       <c r="G130" s="23"/>
@@ -8543,13 +8570,13 @@
     </row>
     <row r="131">
       <c r="C131" s="17" t="s">
-        <v>590</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>367</v>
+        <v>591</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>592</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>368</v>
+        <v>593</v>
       </c>
       <c r="F131" s="23"/>
       <c r="G131" s="23"/>
@@ -8562,13 +8589,13 @@
     </row>
     <row r="132">
       <c r="C132" s="17" t="s">
-        <v>591</v>
-      </c>
-      <c r="D132" s="8" t="s">
-        <v>369</v>
+        <v>594</v>
+      </c>
+      <c r="D132" s="7" t="s">
+        <v>367</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F132" s="23"/>
       <c r="G132" s="23"/>
@@ -8581,13 +8608,13 @@
     </row>
     <row r="133">
       <c r="C133" s="17" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>593</v>
-      </c>
-      <c r="E133" s="8" t="s">
-        <v>594</v>
+        <v>369</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>370</v>
       </c>
       <c r="F133" s="23"/>
       <c r="G133" s="23"/>
@@ -8600,13 +8627,13 @@
     </row>
     <row r="134">
       <c r="C134" s="17" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>333</v>
+        <v>597</v>
       </c>
       <c r="E134" s="8" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="F134" s="23"/>
       <c r="G134" s="23"/>
@@ -8619,13 +8646,13 @@
     </row>
     <row r="135">
       <c r="C135" s="17" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E135" s="8" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="F135" s="23"/>
       <c r="G135" s="23"/>
@@ -8638,13 +8665,13 @@
     </row>
     <row r="136">
       <c r="C136" s="17" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E136" s="8" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="F136" s="23"/>
       <c r="G136" s="23"/>
@@ -8657,13 +8684,13 @@
     </row>
     <row r="137">
       <c r="C137" s="17" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
+      </c>
+      <c r="E137" s="8" t="s">
+        <v>604</v>
       </c>
       <c r="F137" s="23"/>
       <c r="G137" s="23"/>
@@ -8676,13 +8703,13 @@
     </row>
     <row r="138">
       <c r="C138" s="17" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="E138" s="8" t="s">
-        <v>603</v>
+        <v>341</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>342</v>
       </c>
       <c r="F138" s="23"/>
       <c r="G138" s="23"/>
@@ -8695,13 +8722,13 @@
     </row>
     <row r="139">
       <c r="C139" s="17" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="E139" s="3" t="s">
-        <v>605</v>
+        <v>344</v>
+      </c>
+      <c r="E139" s="8" t="s">
+        <v>607</v>
       </c>
       <c r="F139" s="23"/>
       <c r="G139" s="23"/>
@@ -8714,13 +8741,13 @@
     </row>
     <row r="140">
       <c r="C140" s="17" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>357</v>
+        <v>609</v>
       </c>
       <c r="F140" s="23"/>
       <c r="G140" s="23"/>
@@ -8732,14 +8759,14 @@
       <c r="M140" s="23"/>
     </row>
     <row r="141">
-      <c r="C141" s="20" t="s">
-        <v>607</v>
+      <c r="C141" s="17" t="s">
+        <v>610</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="E141" s="4" t="s">
-        <v>363</v>
+        <v>356</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>357</v>
       </c>
       <c r="F141" s="23"/>
       <c r="G141" s="23"/>
@@ -8752,13 +8779,13 @@
     </row>
     <row r="142">
       <c r="C142" s="20" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="E142" s="3" t="s">
-        <v>262</v>
+        <v>362</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>363</v>
       </c>
       <c r="F142" s="23"/>
       <c r="G142" s="23"/>
@@ -8770,20 +8797,14 @@
       <c r="M142" s="23"/>
     </row>
     <row r="143">
-      <c r="A143" s="20" t="s">
-        <v>609</v>
-      </c>
-      <c r="B143" s="20" t="s">
-        <v>396</v>
-      </c>
       <c r="C143" s="20" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="E143" s="8" t="s">
-        <v>274</v>
+        <v>261</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="F143" s="23"/>
       <c r="G143" s="23"/>
@@ -8795,17 +8816,20 @@
       <c r="M143" s="23"/>
     </row>
     <row r="144">
+      <c r="A144" s="20" t="s">
+        <v>613</v>
+      </c>
       <c r="B144" s="20" t="s">
-        <v>454</v>
+        <v>396</v>
       </c>
       <c r="C144" s="20" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="E144" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
+      </c>
+      <c r="E144" s="8" t="s">
+        <v>274</v>
       </c>
       <c r="F144" s="23"/>
       <c r="G144" s="23"/>
@@ -8817,14 +8841,17 @@
       <c r="M144" s="23"/>
     </row>
     <row r="145">
+      <c r="B145" s="20" t="s">
+        <v>454</v>
+      </c>
       <c r="C145" s="20" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="E145" s="8" t="s">
-        <v>613</v>
+        <v>271</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>272</v>
       </c>
       <c r="F145" s="23"/>
       <c r="G145" s="23"/>
@@ -8836,20 +8863,14 @@
       <c r="M145" s="23"/>
     </row>
     <row r="146">
-      <c r="A146" s="20" t="s">
-        <v>614</v>
-      </c>
-      <c r="B146" s="20" t="s">
-        <v>473</v>
-      </c>
       <c r="C146" s="20" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>80</v>
+        <v>275</v>
       </c>
       <c r="E146" s="8" t="s">
-        <v>207</v>
+        <v>617</v>
       </c>
       <c r="F146" s="23"/>
       <c r="G146" s="23"/>
@@ -8861,14 +8882,20 @@
       <c r="M146" s="23"/>
     </row>
     <row r="147">
+      <c r="A147" s="20" t="s">
+        <v>618</v>
+      </c>
+      <c r="B147" s="20" t="s">
+        <v>473</v>
+      </c>
       <c r="C147" s="20" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>92</v>
+        <v>207</v>
       </c>
       <c r="F147" s="23"/>
       <c r="G147" s="23"/>
@@ -8881,13 +8908,13 @@
     </row>
     <row r="148">
       <c r="C148" s="20" t="s">
-        <v>617</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E148" s="3" t="s">
-        <v>618</v>
+        <v>620</v>
+      </c>
+      <c r="D148" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E148" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="F148" s="23"/>
       <c r="G148" s="23"/>
@@ -8899,14 +8926,14 @@
       <c r="M148" s="23"/>
     </row>
     <row r="149">
-      <c r="C149" s="7" t="s">
-        <v>619</v>
+      <c r="C149" s="20" t="s">
+        <v>621</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>620</v>
+        <v>88</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="F149" s="23"/>
       <c r="G149" s="23"/>
@@ -8918,17 +8945,14 @@
       <c r="M149" s="23"/>
     </row>
     <row r="150">
-      <c r="B150" s="20" t="s">
-        <v>396</v>
-      </c>
       <c r="C150" s="7" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>237</v>
+        <v>624</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>211</v>
+        <v>625</v>
       </c>
       <c r="F150" s="23"/>
       <c r="G150" s="23"/>
@@ -8940,14 +8964,17 @@
       <c r="M150" s="23"/>
     </row>
     <row r="151">
+      <c r="B151" s="20" t="s">
+        <v>396</v>
+      </c>
       <c r="C151" s="7" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>365</v>
+        <v>237</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>366</v>
+        <v>211</v>
       </c>
       <c r="F151" s="23"/>
       <c r="G151" s="23"/>
@@ -8960,13 +8987,13 @@
     </row>
     <row r="152">
       <c r="C152" s="7" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>210</v>
+        <v>365</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>83</v>
+        <v>366</v>
       </c>
       <c r="F152" s="23"/>
       <c r="G152" s="23"/>
@@ -8979,13 +9006,13 @@
     </row>
     <row r="153">
       <c r="C153" s="7" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>84</v>
+        <v>210</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>213</v>
+        <v>83</v>
       </c>
       <c r="F153" s="23"/>
       <c r="G153" s="23"/>
@@ -8998,13 +9025,13 @@
     </row>
     <row r="154">
       <c r="C154" s="7" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>216</v>
+        <v>84</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F154" s="23"/>
       <c r="G154" s="23"/>
@@ -9017,13 +9044,13 @@
     </row>
     <row r="155">
       <c r="C155" s="7" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F155" s="23"/>
       <c r="G155" s="23"/>
@@ -9035,17 +9062,14 @@
       <c r="M155" s="23"/>
     </row>
     <row r="156">
-      <c r="B156" s="20" t="s">
-        <v>454</v>
-      </c>
-      <c r="C156" s="20" t="s">
-        <v>628</v>
+      <c r="C156" s="7" t="s">
+        <v>631</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E156" s="7" t="s">
-        <v>256</v>
+        <v>218</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="F156" s="23"/>
       <c r="G156" s="23"/>
@@ -9057,14 +9081,17 @@
       <c r="M156" s="23"/>
     </row>
     <row r="157">
+      <c r="B157" s="20" t="s">
+        <v>454</v>
+      </c>
       <c r="C157" s="20" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>630</v>
+        <v>221</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>256</v>
       </c>
       <c r="F157" s="23"/>
       <c r="G157" s="23"/>
@@ -9077,13 +9104,13 @@
     </row>
     <row r="158">
       <c r="C158" s="20" t="s">
-        <v>631</v>
-      </c>
-      <c r="D158" s="11" t="s">
-        <v>632</v>
-      </c>
-      <c r="E158" s="11" t="s">
         <v>633</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>634</v>
       </c>
       <c r="F158" s="23"/>
       <c r="G158" s="23"/>
@@ -9096,13 +9123,13 @@
     </row>
     <row r="159">
       <c r="C159" s="20" t="s">
-        <v>634</v>
-      </c>
-      <c r="D159" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E159" s="3" t="s">
         <v>635</v>
+      </c>
+      <c r="D159" s="11" t="s">
+        <v>636</v>
+      </c>
+      <c r="E159" s="11" t="s">
+        <v>637</v>
       </c>
       <c r="F159" s="23"/>
       <c r="G159" s="23"/>
@@ -9115,13 +9142,13 @@
     </row>
     <row r="160">
       <c r="C160" s="20" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>236</v>
+        <v>639</v>
       </c>
       <c r="F160" s="23"/>
       <c r="G160" s="23"/>
@@ -9134,13 +9161,13 @@
     </row>
     <row r="161">
       <c r="C161" s="20" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>638</v>
+        <v>236</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>639</v>
+        <v>236</v>
       </c>
       <c r="F161" s="23"/>
       <c r="G161" s="23"/>
@@ -9152,17 +9179,14 @@
       <c r="M161" s="23"/>
     </row>
     <row r="162">
-      <c r="B162" s="20" t="s">
-        <v>437</v>
-      </c>
-      <c r="C162" s="7" t="s">
-        <v>640</v>
+      <c r="C162" s="20" t="s">
+        <v>641</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F162" s="23"/>
       <c r="G162" s="23"/>
@@ -9174,14 +9198,17 @@
       <c r="M162" s="23"/>
     </row>
     <row r="163">
+      <c r="B163" s="20" t="s">
+        <v>437</v>
+      </c>
       <c r="C163" s="7" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F163" s="23"/>
       <c r="G163" s="23"/>
@@ -9194,13 +9221,13 @@
     </row>
     <row r="164">
       <c r="C164" s="7" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="E164" s="7" t="s">
-        <v>240</v>
+        <v>648</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>649</v>
       </c>
       <c r="F164" s="23"/>
       <c r="G164" s="23"/>
@@ -9212,20 +9239,14 @@
       <c r="M164" s="23"/>
     </row>
     <row r="165">
-      <c r="A165" s="20" t="s">
-        <v>647</v>
-      </c>
-      <c r="B165" s="20" t="s">
-        <v>648</v>
-      </c>
-      <c r="C165" s="20" t="s">
-        <v>649</v>
+      <c r="C165" s="7" t="s">
+        <v>650</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>651</v>
+        <v>239</v>
+      </c>
+      <c r="E165" s="7" t="s">
+        <v>240</v>
       </c>
       <c r="F165" s="23"/>
       <c r="G165" s="23"/>
@@ -9237,14 +9258,20 @@
       <c r="M165" s="23"/>
     </row>
     <row r="166">
+      <c r="A166" s="20" t="s">
+        <v>651</v>
+      </c>
+      <c r="B166" s="20" t="s">
+        <v>652</v>
+      </c>
       <c r="C166" s="20" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="E166" s="8" t="s">
         <v>654</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>655</v>
       </c>
       <c r="F166" s="23"/>
       <c r="G166" s="23"/>
@@ -9257,13 +9284,13 @@
     </row>
     <row r="167">
       <c r="C167" s="20" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="E167" s="3" t="s">
         <v>657</v>
+      </c>
+      <c r="E167" s="8" t="s">
+        <v>658</v>
       </c>
       <c r="F167" s="23"/>
       <c r="G167" s="23"/>
@@ -9276,13 +9303,13 @@
     </row>
     <row r="168">
       <c r="C168" s="20" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="F168" s="23"/>
       <c r="G168" s="23"/>
@@ -9294,17 +9321,14 @@
       <c r="M168" s="23"/>
     </row>
     <row r="169">
-      <c r="B169" s="20" t="s">
-        <v>437</v>
-      </c>
       <c r="C169" s="20" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="E169" s="8" t="s">
         <v>663</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>664</v>
       </c>
       <c r="F169" s="23"/>
       <c r="G169" s="23"/>
@@ -9316,14 +9340,17 @@
       <c r="M169" s="23"/>
     </row>
     <row r="170">
+      <c r="B170" s="20" t="s">
+        <v>437</v>
+      </c>
       <c r="C170" s="20" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="F170" s="23"/>
       <c r="G170" s="23"/>
@@ -9335,20 +9362,14 @@
       <c r="M170" s="23"/>
     </row>
     <row r="171">
-      <c r="A171" s="20" t="s">
-        <v>667</v>
-      </c>
-      <c r="B171" s="20" t="s">
-        <v>454</v>
-      </c>
       <c r="C171" s="20" t="s">
         <v>668</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>374</v>
+        <v>669</v>
       </c>
       <c r="E171" s="8" t="s">
-        <v>375</v>
+        <v>670</v>
       </c>
       <c r="F171" s="23"/>
       <c r="G171" s="23"/>
@@ -9360,10 +9381,21 @@
       <c r="M171" s="23"/>
     </row>
     <row r="172">
-      <c r="A172" s="20"/>
-      <c r="B172" s="20"/>
-      <c r="C172" s="20"/>
-      <c r="D172" s="3"/>
+      <c r="A172" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="B172" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="C172" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="E172" s="8" t="s">
+        <v>375</v>
+      </c>
       <c r="F172" s="23"/>
       <c r="G172" s="23"/>
       <c r="H172" s="23"/>
@@ -9376,9 +9408,6 @@
     <row r="173">
       <c r="A173" s="20"/>
       <c r="B173" s="20"/>
-      <c r="C173" s="20"/>
-      <c r="D173" s="3"/>
-      <c r="E173" s="3"/>
       <c r="F173" s="23"/>
       <c r="G173" s="23"/>
       <c r="H173" s="23"/>
@@ -9393,6 +9422,7 @@
       <c r="B174" s="20"/>
       <c r="C174" s="20"/>
       <c r="D174" s="3"/>
+      <c r="E174" s="3"/>
       <c r="F174" s="23"/>
       <c r="G174" s="23"/>
       <c r="H174" s="23"/>
@@ -9406,6 +9436,7 @@
       <c r="A175" s="20"/>
       <c r="B175" s="20"/>
       <c r="C175" s="20"/>
+      <c r="D175" s="3"/>
       <c r="F175" s="23"/>
       <c r="G175" s="23"/>
       <c r="H175" s="23"/>
@@ -9419,7 +9450,6 @@
       <c r="A176" s="20"/>
       <c r="B176" s="20"/>
       <c r="C176" s="20"/>
-      <c r="D176" s="3"/>
       <c r="F176" s="23"/>
       <c r="G176" s="23"/>
       <c r="H176" s="23"/>
@@ -9433,6 +9463,7 @@
       <c r="A177" s="20"/>
       <c r="B177" s="20"/>
       <c r="C177" s="20"/>
+      <c r="D177" s="3"/>
       <c r="F177" s="23"/>
       <c r="G177" s="23"/>
       <c r="H177" s="23"/>
@@ -9545,6 +9576,19 @@
       <c r="K185" s="23"/>
       <c r="L185" s="23"/>
       <c r="M185" s="23"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="20"/>
+      <c r="B186" s="20"/>
+      <c r="C186" s="20"/>
+      <c r="F186" s="23"/>
+      <c r="G186" s="23"/>
+      <c r="H186" s="23"/>
+      <c r="I186" s="23"/>
+      <c r="J186" s="23"/>
+      <c r="K186" s="23"/>
+      <c r="L186" s="23"/>
+      <c r="M186" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="34">
@@ -9564,24 +9608,24 @@
     <mergeCell ref="A70:A80"/>
     <mergeCell ref="B70:B76"/>
     <mergeCell ref="A81:A85"/>
-    <mergeCell ref="A116:A142"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A146:A164"/>
-    <mergeCell ref="A165:A170"/>
-    <mergeCell ref="B144:B145"/>
-    <mergeCell ref="B146:B149"/>
-    <mergeCell ref="B150:B155"/>
-    <mergeCell ref="B156:B161"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="B165:B168"/>
-    <mergeCell ref="B169:B170"/>
-    <mergeCell ref="A97:A115"/>
+    <mergeCell ref="A117:A143"/>
+    <mergeCell ref="A144:A146"/>
+    <mergeCell ref="A147:A165"/>
+    <mergeCell ref="A166:A171"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="B147:B150"/>
+    <mergeCell ref="B151:B156"/>
+    <mergeCell ref="B157:B162"/>
+    <mergeCell ref="B163:B165"/>
+    <mergeCell ref="B166:B169"/>
+    <mergeCell ref="B170:B171"/>
     <mergeCell ref="B97:B98"/>
     <mergeCell ref="B101:B113"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="B116:B124"/>
-    <mergeCell ref="B125:B128"/>
-    <mergeCell ref="B129:B142"/>
+    <mergeCell ref="B130:B143"/>
+    <mergeCell ref="A97:A116"/>
+    <mergeCell ref="B126:B129"/>
+    <mergeCell ref="B117:B125"/>
+    <mergeCell ref="B115:B116"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor:shared link access (#213)
* feat: apply new i18n for copy and copied in share link

* chore: comment for sharedURl

* fix: type error
</commit_message>
<xml_diff>
--- a/scripts/i18n.xlsx
+++ b/scripts/i18n.xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1228" uniqueCount="669">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="673">
   <si>
     <t xml:space="preserve">페이지는 [피그마] PFPlay GUI 설계서 합본의 페이지 이름입니다. </t>
   </si>
@@ -1843,6 +1843,9 @@
     <t>party.para.copy_completed</t>
   </si>
   <si>
+    <t>Copied!</t>
+  </si>
+  <si>
     <t>party.para.close_party</t>
   </si>
   <si>
@@ -1882,10 +1885,19 @@
     <t>party.para.enter_confirm_phrase</t>
   </si>
   <si>
+    <t>party.para.share_x_partyroom</t>
+  </si>
+  <si>
+    <t>I'm listening to the {partyroom_name} room. Come hang out!</t>
+  </si>
+  <si>
     <t>party.btn.share_twitter</t>
   </si>
   <si>
     <t>party.btn.copy_link</t>
+  </si>
+  <si>
+    <t>Copy</t>
   </si>
   <si>
     <t>디제잉 (DJ)</t>
@@ -2205,7 +2217,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -2251,11 +2263,16 @@
       <name val="&quot;Google Sans&quot;"/>
     </font>
     <font>
+      <sz val="11.0"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="NotoSansKR"/>
+    </font>
+    <font>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2280,6 +2297,12 @@
         <bgColor rgb="FF282C34"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F8F8"/>
+        <bgColor rgb="FFF8F8F8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border/>
@@ -2287,7 +2310,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2378,7 +2401,10 @@
     <xf quotePrefix="1" borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="5" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -8059,7 +8085,7 @@
         <v>171</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>172</v>
+        <v>550</v>
       </c>
       <c r="F106" s="23"/>
       <c r="G106" s="28"/>
@@ -8072,13 +8098,13 @@
     </row>
     <row r="107">
       <c r="C107" s="20" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F107" s="23"/>
       <c r="G107" s="28"/>
@@ -8091,13 +8117,13 @@
     </row>
     <row r="108">
       <c r="C108" s="20" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="D108" s="29" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="F108" s="23"/>
       <c r="G108" s="28"/>
@@ -8110,7 +8136,7 @@
     </row>
     <row r="109">
       <c r="C109" s="20" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>287</v>
@@ -8129,7 +8155,7 @@
     </row>
     <row r="110">
       <c r="C110" s="20" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="D110" s="20" t="s">
         <v>281</v>
@@ -8148,13 +8174,13 @@
     </row>
     <row r="111">
       <c r="C111" s="20" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="D111" s="20" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="E111" s="20" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="F111" s="23"/>
       <c r="G111" s="28"/>
@@ -8167,7 +8193,7 @@
     </row>
     <row r="112">
       <c r="C112" s="20" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="D112" s="8" t="s">
         <v>197</v>
@@ -8186,7 +8212,7 @@
     </row>
     <row r="113">
       <c r="C113" s="20" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="D113" s="8" t="s">
         <v>199</v>
@@ -8204,17 +8230,15 @@
       <c r="M113" s="27"/>
     </row>
     <row r="114">
-      <c r="B114" s="20" t="s">
-        <v>396</v>
-      </c>
+      <c r="B114" s="20"/>
       <c r="C114" s="20" t="s">
-        <v>563</v>
-      </c>
-      <c r="D114" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E114" s="3" t="s">
-        <v>168</v>
+        <v>564</v>
+      </c>
+      <c r="D114" s="30" t="s">
+        <v>565</v>
+      </c>
+      <c r="E114" s="30" t="s">
+        <v>565</v>
       </c>
       <c r="F114" s="23"/>
       <c r="G114" s="28"/>
@@ -8226,14 +8250,17 @@
       <c r="M114" s="27"/>
     </row>
     <row r="115">
+      <c r="B115" s="20" t="s">
+        <v>396</v>
+      </c>
       <c r="C115" s="20" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F115" s="23"/>
       <c r="G115" s="28"/>
@@ -8245,20 +8272,14 @@
       <c r="M115" s="27"/>
     </row>
     <row r="116">
-      <c r="A116" s="17" t="s">
-        <v>565</v>
-      </c>
-      <c r="B116" s="17" t="s">
-        <v>473</v>
-      </c>
-      <c r="C116" s="17" t="s">
-        <v>566</v>
+      <c r="C116" s="20" t="s">
+        <v>567</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>314</v>
+        <v>568</v>
       </c>
       <c r="F116" s="23"/>
       <c r="G116" s="28"/>
@@ -8270,55 +8291,61 @@
       <c r="M116" s="27"/>
     </row>
     <row r="117">
+      <c r="A117" s="17" t="s">
+        <v>569</v>
+      </c>
+      <c r="B117" s="17" t="s">
+        <v>473</v>
+      </c>
       <c r="C117" s="17" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>111</v>
+        <v>314</v>
       </c>
       <c r="F117" s="23"/>
       <c r="G117" s="28"/>
       <c r="H117" s="26"/>
       <c r="I117" s="25"/>
       <c r="J117" s="25"/>
-      <c r="K117" s="23"/>
-      <c r="L117" s="23"/>
-      <c r="M117" s="23"/>
+      <c r="K117" s="27"/>
+      <c r="L117" s="27"/>
+      <c r="M117" s="27"/>
     </row>
     <row r="118">
       <c r="C118" s="17" t="s">
-        <v>568</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>569</v>
-      </c>
-      <c r="E118" s="8" t="s">
-        <v>570</v>
+        <v>571</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>111</v>
       </c>
       <c r="F118" s="23"/>
-      <c r="G118" s="30"/>
-      <c r="H118" s="23"/>
-      <c r="I118" s="23"/>
-      <c r="J118" s="23"/>
+      <c r="G118" s="28"/>
+      <c r="H118" s="26"/>
+      <c r="I118" s="25"/>
+      <c r="J118" s="25"/>
       <c r="K118" s="23"/>
       <c r="L118" s="23"/>
       <c r="M118" s="23"/>
     </row>
     <row r="119">
-      <c r="C119" s="20" t="s">
-        <v>571</v>
+      <c r="C119" s="17" t="s">
+        <v>572</v>
       </c>
       <c r="D119" s="8" t="s">
-        <v>354</v>
+        <v>573</v>
       </c>
       <c r="E119" s="8" t="s">
-        <v>355</v>
+        <v>574</v>
       </c>
       <c r="F119" s="23"/>
-      <c r="G119" s="23"/>
+      <c r="G119" s="31"/>
       <c r="H119" s="23"/>
       <c r="I119" s="23"/>
       <c r="J119" s="23"/>
@@ -8327,14 +8354,14 @@
       <c r="M119" s="23"/>
     </row>
     <row r="120">
-      <c r="C120" s="17" t="s">
-        <v>572</v>
+      <c r="C120" s="20" t="s">
+        <v>575</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>137</v>
+        <v>354</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>138</v>
+        <v>355</v>
       </c>
       <c r="F120" s="23"/>
       <c r="G120" s="23"/>
@@ -8347,13 +8374,13 @@
     </row>
     <row r="121">
       <c r="C121" s="17" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="F121" s="23"/>
       <c r="G121" s="23"/>
@@ -8366,13 +8393,13 @@
     </row>
     <row r="122">
       <c r="C122" s="17" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="D122" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E122" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F122" s="23"/>
       <c r="G122" s="23"/>
@@ -8385,13 +8412,13 @@
     </row>
     <row r="123">
       <c r="C123" s="17" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F123" s="23"/>
       <c r="G123" s="23"/>
@@ -8404,13 +8431,13 @@
     </row>
     <row r="124">
       <c r="C124" s="17" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="F124" s="23"/>
       <c r="G124" s="23"/>
@@ -8422,17 +8449,14 @@
       <c r="M124" s="23"/>
     </row>
     <row r="125">
-      <c r="B125" s="17" t="s">
-        <v>396</v>
-      </c>
       <c r="C125" s="17" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="D125" s="8" t="s">
-        <v>317</v>
+        <v>117</v>
       </c>
       <c r="E125" s="8" t="s">
-        <v>578</v>
+        <v>118</v>
       </c>
       <c r="F125" s="23"/>
       <c r="G125" s="23"/>
@@ -8444,14 +8468,17 @@
       <c r="M125" s="23"/>
     </row>
     <row r="126">
+      <c r="B126" s="17" t="s">
+        <v>396</v>
+      </c>
       <c r="C126" s="17" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="D126" s="8" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E126" s="8" t="s">
-        <v>324</v>
+        <v>582</v>
       </c>
       <c r="F126" s="23"/>
       <c r="G126" s="23"/>
@@ -8463,14 +8490,14 @@
       <c r="M126" s="23"/>
     </row>
     <row r="127">
-      <c r="C127" s="31" t="s">
-        <v>580</v>
+      <c r="C127" s="17" t="s">
+        <v>583</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>351</v>
+        <v>323</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>581</v>
+        <v>324</v>
       </c>
       <c r="F127" s="23"/>
       <c r="G127" s="23"/>
@@ -8482,14 +8509,14 @@
       <c r="M127" s="23"/>
     </row>
     <row r="128">
-      <c r="C128" s="17" t="s">
-        <v>582</v>
+      <c r="C128" s="32" t="s">
+        <v>584</v>
       </c>
       <c r="D128" s="8" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="F128" s="23"/>
       <c r="G128" s="23"/>
@@ -8501,17 +8528,14 @@
       <c r="M128" s="23"/>
     </row>
     <row r="129">
-      <c r="B129" s="17" t="s">
-        <v>454</v>
-      </c>
       <c r="C129" s="17" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
       <c r="D129" s="8" t="s">
-        <v>585</v>
+        <v>347</v>
       </c>
       <c r="E129" s="8" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="F129" s="23"/>
       <c r="G129" s="23"/>
@@ -8523,14 +8547,17 @@
       <c r="M129" s="23"/>
     </row>
     <row r="130">
+      <c r="B130" s="17" t="s">
+        <v>454</v>
+      </c>
       <c r="C130" s="17" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="D130" s="8" t="s">
-        <v>588</v>
-      </c>
-      <c r="E130" s="3" t="s">
         <v>589</v>
+      </c>
+      <c r="E130" s="8" t="s">
+        <v>590</v>
       </c>
       <c r="F130" s="23"/>
       <c r="G130" s="23"/>
@@ -8543,13 +8570,13 @@
     </row>
     <row r="131">
       <c r="C131" s="17" t="s">
-        <v>590</v>
-      </c>
-      <c r="D131" s="7" t="s">
-        <v>367</v>
+        <v>591</v>
+      </c>
+      <c r="D131" s="8" t="s">
+        <v>592</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>368</v>
+        <v>593</v>
       </c>
       <c r="F131" s="23"/>
       <c r="G131" s="23"/>
@@ -8562,13 +8589,13 @@
     </row>
     <row r="132">
       <c r="C132" s="17" t="s">
-        <v>591</v>
-      </c>
-      <c r="D132" s="8" t="s">
-        <v>369</v>
+        <v>594</v>
+      </c>
+      <c r="D132" s="7" t="s">
+        <v>367</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="F132" s="23"/>
       <c r="G132" s="23"/>
@@ -8581,13 +8608,13 @@
     </row>
     <row r="133">
       <c r="C133" s="17" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="D133" s="8" t="s">
-        <v>593</v>
-      </c>
-      <c r="E133" s="8" t="s">
-        <v>594</v>
+        <v>369</v>
+      </c>
+      <c r="E133" s="3" t="s">
+        <v>370</v>
       </c>
       <c r="F133" s="23"/>
       <c r="G133" s="23"/>
@@ -8600,13 +8627,13 @@
     </row>
     <row r="134">
       <c r="C134" s="17" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="D134" s="8" t="s">
-        <v>333</v>
+        <v>597</v>
       </c>
       <c r="E134" s="8" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="F134" s="23"/>
       <c r="G134" s="23"/>
@@ -8619,13 +8646,13 @@
     </row>
     <row r="135">
       <c r="C135" s="17" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="D135" s="8" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="E135" s="8" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="F135" s="23"/>
       <c r="G135" s="23"/>
@@ -8638,13 +8665,13 @@
     </row>
     <row r="136">
       <c r="C136" s="17" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="E136" s="8" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="F136" s="23"/>
       <c r="G136" s="23"/>
@@ -8657,13 +8684,13 @@
     </row>
     <row r="137">
       <c r="C137" s="17" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="D137" s="8" t="s">
-        <v>341</v>
-      </c>
-      <c r="E137" s="3" t="s">
-        <v>342</v>
+        <v>338</v>
+      </c>
+      <c r="E137" s="8" t="s">
+        <v>604</v>
       </c>
       <c r="F137" s="23"/>
       <c r="G137" s="23"/>
@@ -8676,13 +8703,13 @@
     </row>
     <row r="138">
       <c r="C138" s="17" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="D138" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="E138" s="8" t="s">
-        <v>603</v>
+        <v>341</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>342</v>
       </c>
       <c r="F138" s="23"/>
       <c r="G138" s="23"/>
@@ -8695,13 +8722,13 @@
     </row>
     <row r="139">
       <c r="C139" s="17" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="D139" s="8" t="s">
-        <v>349</v>
-      </c>
-      <c r="E139" s="3" t="s">
-        <v>605</v>
+        <v>344</v>
+      </c>
+      <c r="E139" s="8" t="s">
+        <v>607</v>
       </c>
       <c r="F139" s="23"/>
       <c r="G139" s="23"/>
@@ -8714,13 +8741,13 @@
     </row>
     <row r="140">
       <c r="C140" s="17" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="D140" s="8" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>357</v>
+        <v>609</v>
       </c>
       <c r="F140" s="23"/>
       <c r="G140" s="23"/>
@@ -8732,14 +8759,14 @@
       <c r="M140" s="23"/>
     </row>
     <row r="141">
-      <c r="C141" s="20" t="s">
-        <v>607</v>
+      <c r="C141" s="17" t="s">
+        <v>610</v>
       </c>
       <c r="D141" s="8" t="s">
-        <v>362</v>
-      </c>
-      <c r="E141" s="4" t="s">
-        <v>363</v>
+        <v>356</v>
+      </c>
+      <c r="E141" s="3" t="s">
+        <v>357</v>
       </c>
       <c r="F141" s="23"/>
       <c r="G141" s="23"/>
@@ -8752,13 +8779,13 @@
     </row>
     <row r="142">
       <c r="C142" s="20" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="D142" s="8" t="s">
-        <v>261</v>
-      </c>
-      <c r="E142" s="3" t="s">
-        <v>262</v>
+        <v>362</v>
+      </c>
+      <c r="E142" s="4" t="s">
+        <v>363</v>
       </c>
       <c r="F142" s="23"/>
       <c r="G142" s="23"/>
@@ -8770,20 +8797,14 @@
       <c r="M142" s="23"/>
     </row>
     <row r="143">
-      <c r="A143" s="20" t="s">
-        <v>609</v>
-      </c>
-      <c r="B143" s="20" t="s">
-        <v>396</v>
-      </c>
       <c r="C143" s="20" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="D143" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="E143" s="8" t="s">
-        <v>274</v>
+        <v>261</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>262</v>
       </c>
       <c r="F143" s="23"/>
       <c r="G143" s="23"/>
@@ -8795,17 +8816,20 @@
       <c r="M143" s="23"/>
     </row>
     <row r="144">
+      <c r="A144" s="20" t="s">
+        <v>613</v>
+      </c>
       <c r="B144" s="20" t="s">
-        <v>454</v>
+        <v>396</v>
       </c>
       <c r="C144" s="20" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="D144" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="E144" s="3" t="s">
-        <v>272</v>
+        <v>273</v>
+      </c>
+      <c r="E144" s="8" t="s">
+        <v>274</v>
       </c>
       <c r="F144" s="23"/>
       <c r="G144" s="23"/>
@@ -8817,14 +8841,17 @@
       <c r="M144" s="23"/>
     </row>
     <row r="145">
+      <c r="B145" s="20" t="s">
+        <v>454</v>
+      </c>
       <c r="C145" s="20" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="D145" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="E145" s="8" t="s">
-        <v>613</v>
+        <v>271</v>
+      </c>
+      <c r="E145" s="3" t="s">
+        <v>272</v>
       </c>
       <c r="F145" s="23"/>
       <c r="G145" s="23"/>
@@ -8836,20 +8863,14 @@
       <c r="M145" s="23"/>
     </row>
     <row r="146">
-      <c r="A146" s="20" t="s">
-        <v>614</v>
-      </c>
-      <c r="B146" s="20" t="s">
-        <v>473</v>
-      </c>
       <c r="C146" s="20" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="D146" s="8" t="s">
-        <v>80</v>
+        <v>275</v>
       </c>
       <c r="E146" s="8" t="s">
-        <v>207</v>
+        <v>617</v>
       </c>
       <c r="F146" s="23"/>
       <c r="G146" s="23"/>
@@ -8861,14 +8882,20 @@
       <c r="M146" s="23"/>
     </row>
     <row r="147">
+      <c r="A147" s="20" t="s">
+        <v>618</v>
+      </c>
+      <c r="B147" s="20" t="s">
+        <v>473</v>
+      </c>
       <c r="C147" s="20" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>92</v>
+        <v>207</v>
       </c>
       <c r="F147" s="23"/>
       <c r="G147" s="23"/>
@@ -8881,13 +8908,13 @@
     </row>
     <row r="148">
       <c r="C148" s="20" t="s">
-        <v>617</v>
-      </c>
-      <c r="D148" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E148" s="3" t="s">
-        <v>618</v>
+        <v>620</v>
+      </c>
+      <c r="D148" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E148" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="F148" s="23"/>
       <c r="G148" s="23"/>
@@ -8899,14 +8926,14 @@
       <c r="M148" s="23"/>
     </row>
     <row r="149">
-      <c r="C149" s="7" t="s">
-        <v>619</v>
+      <c r="C149" s="20" t="s">
+        <v>621</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>620</v>
+        <v>88</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="F149" s="23"/>
       <c r="G149" s="23"/>
@@ -8918,17 +8945,14 @@
       <c r="M149" s="23"/>
     </row>
     <row r="150">
-      <c r="B150" s="20" t="s">
-        <v>396</v>
-      </c>
       <c r="C150" s="7" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>237</v>
+        <v>624</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>211</v>
+        <v>625</v>
       </c>
       <c r="F150" s="23"/>
       <c r="G150" s="23"/>
@@ -8940,14 +8964,17 @@
       <c r="M150" s="23"/>
     </row>
     <row r="151">
+      <c r="B151" s="20" t="s">
+        <v>396</v>
+      </c>
       <c r="C151" s="7" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>365</v>
+        <v>237</v>
       </c>
       <c r="E151" s="3" t="s">
-        <v>366</v>
+        <v>211</v>
       </c>
       <c r="F151" s="23"/>
       <c r="G151" s="23"/>
@@ -8960,13 +8987,13 @@
     </row>
     <row r="152">
       <c r="C152" s="7" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>210</v>
+        <v>365</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>83</v>
+        <v>366</v>
       </c>
       <c r="F152" s="23"/>
       <c r="G152" s="23"/>
@@ -8979,13 +9006,13 @@
     </row>
     <row r="153">
       <c r="C153" s="7" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>84</v>
+        <v>210</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>213</v>
+        <v>83</v>
       </c>
       <c r="F153" s="23"/>
       <c r="G153" s="23"/>
@@ -8998,13 +9025,13 @@
     </row>
     <row r="154">
       <c r="C154" s="7" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>216</v>
+        <v>84</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="F154" s="23"/>
       <c r="G154" s="23"/>
@@ -9017,13 +9044,13 @@
     </row>
     <row r="155">
       <c r="C155" s="7" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="F155" s="23"/>
       <c r="G155" s="23"/>
@@ -9035,17 +9062,14 @@
       <c r="M155" s="23"/>
     </row>
     <row r="156">
-      <c r="B156" s="20" t="s">
-        <v>454</v>
-      </c>
-      <c r="C156" s="20" t="s">
-        <v>628</v>
+      <c r="C156" s="7" t="s">
+        <v>631</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="E156" s="7" t="s">
-        <v>256</v>
+        <v>218</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>219</v>
       </c>
       <c r="F156" s="23"/>
       <c r="G156" s="23"/>
@@ -9057,14 +9081,17 @@
       <c r="M156" s="23"/>
     </row>
     <row r="157">
+      <c r="B157" s="20" t="s">
+        <v>454</v>
+      </c>
       <c r="C157" s="20" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="E157" s="3" t="s">
-        <v>630</v>
+        <v>221</v>
+      </c>
+      <c r="E157" s="7" t="s">
+        <v>256</v>
       </c>
       <c r="F157" s="23"/>
       <c r="G157" s="23"/>
@@ -9077,13 +9104,13 @@
     </row>
     <row r="158">
       <c r="C158" s="20" t="s">
-        <v>631</v>
-      </c>
-      <c r="D158" s="11" t="s">
-        <v>632</v>
-      </c>
-      <c r="E158" s="11" t="s">
         <v>633</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>634</v>
       </c>
       <c r="F158" s="23"/>
       <c r="G158" s="23"/>
@@ -9096,13 +9123,13 @@
     </row>
     <row r="159">
       <c r="C159" s="20" t="s">
-        <v>634</v>
-      </c>
-      <c r="D159" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E159" s="3" t="s">
         <v>635</v>
+      </c>
+      <c r="D159" s="11" t="s">
+        <v>636</v>
+      </c>
+      <c r="E159" s="11" t="s">
+        <v>637</v>
       </c>
       <c r="F159" s="23"/>
       <c r="G159" s="23"/>
@@ -9115,13 +9142,13 @@
     </row>
     <row r="160">
       <c r="C160" s="20" t="s">
-        <v>636</v>
+        <v>638</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>236</v>
+        <v>639</v>
       </c>
       <c r="F160" s="23"/>
       <c r="G160" s="23"/>
@@ -9134,13 +9161,13 @@
     </row>
     <row r="161">
       <c r="C161" s="20" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>638</v>
+        <v>236</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>639</v>
+        <v>236</v>
       </c>
       <c r="F161" s="23"/>
       <c r="G161" s="23"/>
@@ -9152,17 +9179,14 @@
       <c r="M161" s="23"/>
     </row>
     <row r="162">
-      <c r="B162" s="20" t="s">
-        <v>437</v>
-      </c>
-      <c r="C162" s="7" t="s">
-        <v>640</v>
+      <c r="C162" s="20" t="s">
+        <v>641</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="F162" s="23"/>
       <c r="G162" s="23"/>
@@ -9174,14 +9198,17 @@
       <c r="M162" s="23"/>
     </row>
     <row r="163">
+      <c r="B163" s="20" t="s">
+        <v>437</v>
+      </c>
       <c r="C163" s="7" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F163" s="23"/>
       <c r="G163" s="23"/>
@@ -9194,13 +9221,13 @@
     </row>
     <row r="164">
       <c r="C164" s="7" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="E164" s="7" t="s">
-        <v>240</v>
+        <v>648</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>649</v>
       </c>
       <c r="F164" s="23"/>
       <c r="G164" s="23"/>
@@ -9212,20 +9239,14 @@
       <c r="M164" s="23"/>
     </row>
     <row r="165">
-      <c r="A165" s="20" t="s">
-        <v>647</v>
-      </c>
-      <c r="B165" s="20" t="s">
-        <v>648</v>
-      </c>
-      <c r="C165" s="20" t="s">
-        <v>649</v>
+      <c r="C165" s="7" t="s">
+        <v>650</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="E165" s="3" t="s">
-        <v>651</v>
+        <v>239</v>
+      </c>
+      <c r="E165" s="7" t="s">
+        <v>240</v>
       </c>
       <c r="F165" s="23"/>
       <c r="G165" s="23"/>
@@ -9237,14 +9258,20 @@
       <c r="M165" s="23"/>
     </row>
     <row r="166">
+      <c r="A166" s="20" t="s">
+        <v>651</v>
+      </c>
+      <c r="B166" s="20" t="s">
+        <v>652</v>
+      </c>
       <c r="C166" s="20" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="E166" s="8" t="s">
         <v>654</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>655</v>
       </c>
       <c r="F166" s="23"/>
       <c r="G166" s="23"/>
@@ -9257,13 +9284,13 @@
     </row>
     <row r="167">
       <c r="C167" s="20" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="E167" s="3" t="s">
         <v>657</v>
+      </c>
+      <c r="E167" s="8" t="s">
+        <v>658</v>
       </c>
       <c r="F167" s="23"/>
       <c r="G167" s="23"/>
@@ -9276,13 +9303,13 @@
     </row>
     <row r="168">
       <c r="C168" s="20" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="F168" s="23"/>
       <c r="G168" s="23"/>
@@ -9294,17 +9321,14 @@
       <c r="M168" s="23"/>
     </row>
     <row r="169">
-      <c r="B169" s="20" t="s">
-        <v>437</v>
-      </c>
       <c r="C169" s="20" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="E169" s="8" t="s">
         <v>663</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>664</v>
       </c>
       <c r="F169" s="23"/>
       <c r="G169" s="23"/>
@@ -9316,14 +9340,17 @@
       <c r="M169" s="23"/>
     </row>
     <row r="170">
+      <c r="B170" s="20" t="s">
+        <v>437</v>
+      </c>
       <c r="C170" s="20" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="E170" s="8" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="F170" s="23"/>
       <c r="G170" s="23"/>
@@ -9335,20 +9362,14 @@
       <c r="M170" s="23"/>
     </row>
     <row r="171">
-      <c r="A171" s="20" t="s">
-        <v>667</v>
-      </c>
-      <c r="B171" s="20" t="s">
-        <v>454</v>
-      </c>
       <c r="C171" s="20" t="s">
         <v>668</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>374</v>
+        <v>669</v>
       </c>
       <c r="E171" s="8" t="s">
-        <v>375</v>
+        <v>670</v>
       </c>
       <c r="F171" s="23"/>
       <c r="G171" s="23"/>
@@ -9360,10 +9381,21 @@
       <c r="M171" s="23"/>
     </row>
     <row r="172">
-      <c r="A172" s="20"/>
-      <c r="B172" s="20"/>
-      <c r="C172" s="20"/>
-      <c r="D172" s="3"/>
+      <c r="A172" s="20" t="s">
+        <v>671</v>
+      </c>
+      <c r="B172" s="20" t="s">
+        <v>454</v>
+      </c>
+      <c r="C172" s="20" t="s">
+        <v>672</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="E172" s="8" t="s">
+        <v>375</v>
+      </c>
       <c r="F172" s="23"/>
       <c r="G172" s="23"/>
       <c r="H172" s="23"/>
@@ -9376,9 +9408,6 @@
     <row r="173">
       <c r="A173" s="20"/>
       <c r="B173" s="20"/>
-      <c r="C173" s="20"/>
-      <c r="D173" s="3"/>
-      <c r="E173" s="3"/>
       <c r="F173" s="23"/>
       <c r="G173" s="23"/>
       <c r="H173" s="23"/>
@@ -9393,6 +9422,7 @@
       <c r="B174" s="20"/>
       <c r="C174" s="20"/>
       <c r="D174" s="3"/>
+      <c r="E174" s="3"/>
       <c r="F174" s="23"/>
       <c r="G174" s="23"/>
       <c r="H174" s="23"/>
@@ -9406,6 +9436,7 @@
       <c r="A175" s="20"/>
       <c r="B175" s="20"/>
       <c r="C175" s="20"/>
+      <c r="D175" s="3"/>
       <c r="F175" s="23"/>
       <c r="G175" s="23"/>
       <c r="H175" s="23"/>
@@ -9419,7 +9450,6 @@
       <c r="A176" s="20"/>
       <c r="B176" s="20"/>
       <c r="C176" s="20"/>
-      <c r="D176" s="3"/>
       <c r="F176" s="23"/>
       <c r="G176" s="23"/>
       <c r="H176" s="23"/>
@@ -9433,6 +9463,7 @@
       <c r="A177" s="20"/>
       <c r="B177" s="20"/>
       <c r="C177" s="20"/>
+      <c r="D177" s="3"/>
       <c r="F177" s="23"/>
       <c r="G177" s="23"/>
       <c r="H177" s="23"/>
@@ -9545,6 +9576,19 @@
       <c r="K185" s="23"/>
       <c r="L185" s="23"/>
       <c r="M185" s="23"/>
+    </row>
+    <row r="186">
+      <c r="A186" s="20"/>
+      <c r="B186" s="20"/>
+      <c r="C186" s="20"/>
+      <c r="F186" s="23"/>
+      <c r="G186" s="23"/>
+      <c r="H186" s="23"/>
+      <c r="I186" s="23"/>
+      <c r="J186" s="23"/>
+      <c r="K186" s="23"/>
+      <c r="L186" s="23"/>
+      <c r="M186" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="34">
@@ -9564,24 +9608,24 @@
     <mergeCell ref="A70:A80"/>
     <mergeCell ref="B70:B76"/>
     <mergeCell ref="A81:A85"/>
-    <mergeCell ref="A116:A142"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A146:A164"/>
-    <mergeCell ref="A165:A170"/>
-    <mergeCell ref="B144:B145"/>
-    <mergeCell ref="B146:B149"/>
-    <mergeCell ref="B150:B155"/>
-    <mergeCell ref="B156:B161"/>
-    <mergeCell ref="B162:B164"/>
-    <mergeCell ref="B165:B168"/>
-    <mergeCell ref="B169:B170"/>
-    <mergeCell ref="A97:A115"/>
+    <mergeCell ref="A117:A143"/>
+    <mergeCell ref="A144:A146"/>
+    <mergeCell ref="A147:A165"/>
+    <mergeCell ref="A166:A171"/>
+    <mergeCell ref="B145:B146"/>
+    <mergeCell ref="B147:B150"/>
+    <mergeCell ref="B151:B156"/>
+    <mergeCell ref="B157:B162"/>
+    <mergeCell ref="B163:B165"/>
+    <mergeCell ref="B166:B169"/>
+    <mergeCell ref="B170:B171"/>
     <mergeCell ref="B97:B98"/>
     <mergeCell ref="B101:B113"/>
-    <mergeCell ref="B114:B115"/>
-    <mergeCell ref="B116:B124"/>
-    <mergeCell ref="B125:B128"/>
-    <mergeCell ref="B129:B142"/>
+    <mergeCell ref="B130:B143"/>
+    <mergeCell ref="A97:A116"/>
+    <mergeCell ref="B126:B129"/>
+    <mergeCell ref="B117:B125"/>
+    <mergeCell ref="B115:B116"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>